<commit_message>
Changes to python script and excel files
</commit_message>
<xml_diff>
--- a/milestones-consolidated.xlsx
+++ b/milestones-consolidated.xlsx
@@ -648,18 +648,6 @@
     <t>histone modifications\number</t>
   </si>
   <si>
-    <t>2\iPSC, differentiated</t>
-  </si>
-  <si>
-    <t>12\iPSC, differentiated</t>
-  </si>
-  <si>
-    <t>39\iPSC, differentiated</t>
-  </si>
-  <si>
-    <t>12\iPSC, differentiated;12\mature motor neurons</t>
-  </si>
-  <si>
     <t>Broad-Golub</t>
   </si>
   <si>
@@ -750,33 +738,6 @@
     <t>count\type (OR) count1\type1;count2\type2</t>
   </si>
   <si>
-    <t>3\cell line</t>
-  </si>
-  <si>
-    <t>1\cell line;2\iPSC, differentiated</t>
-  </si>
-  <si>
-    <t>4\cell line</t>
-  </si>
-  <si>
-    <t>2\cell line</t>
-  </si>
-  <si>
-    <t>10\cell line</t>
-  </si>
-  <si>
-    <t>6\cell line</t>
-  </si>
-  <si>
-    <t>7\cell line</t>
-  </si>
-  <si>
-    <t>1\cell line</t>
-  </si>
-  <si>
-    <t>5\cell line</t>
-  </si>
-  <si>
     <t>ISMMS-Iyengar</t>
   </si>
   <si>
@@ -802,6 +763,45 @@
   </si>
   <si>
     <t>c-Jun, p-cJun, Foxo3a, p-Stat3, NFkB, and other target proteins</t>
+  </si>
+  <si>
+    <t>3\cell lines</t>
+  </si>
+  <si>
+    <t>1\cell lines;2\iPSCs, differentiated</t>
+  </si>
+  <si>
+    <t>2\iPSCs, differentiated</t>
+  </si>
+  <si>
+    <t>4\cell lines</t>
+  </si>
+  <si>
+    <t>6\cell lines</t>
+  </si>
+  <si>
+    <t>7\cell lines</t>
+  </si>
+  <si>
+    <t>2\cell lines</t>
+  </si>
+  <si>
+    <t>10\cell lines</t>
+  </si>
+  <si>
+    <t>1\cell lines</t>
+  </si>
+  <si>
+    <t>5\cell lines</t>
+  </si>
+  <si>
+    <t>12\iPSCs, differentiated</t>
+  </si>
+  <si>
+    <t>39\iPSCs, differentiated</t>
+  </si>
+  <si>
+    <t>12\iPSCs, differentiated;12\mature motor neurons</t>
   </si>
 </sst>
 </file>
@@ -938,7 +938,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="637">
+  <cellStyleXfs count="641">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1462,6 +1462,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1628,7 +1632,7 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="637">
+  <cellStyles count="641">
     <cellStyle name="Bad" xfId="43" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1946,6 +1950,8 @@
     <cellStyle name="Followed Hyperlink" xfId="632" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="634" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="636" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="638" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="640" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2262,6 +2268,8 @@
     <cellStyle name="Hyperlink" xfId="631" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="633" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="635" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="637" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="639" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="377" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="140"/>
@@ -2604,8 +2612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J33" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="O63" sqref="O63"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0"/>
@@ -2692,10 +2700,10 @@
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>18</v>
@@ -2755,7 +2763,7 @@
     </row>
     <row r="4" spans="1:21" ht="17" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>23</v>
@@ -2764,10 +2772,10 @@
         <v>28</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>29</v>
@@ -2807,7 +2815,7 @@
     </row>
     <row r="5" spans="1:21" ht="17" customHeight="1">
       <c r="A5" s="9" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>24</v>
@@ -2816,10 +2824,10 @@
         <v>28</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>29</v>
@@ -2859,7 +2867,7 @@
     </row>
     <row r="6" spans="1:21" ht="17" customHeight="1">
       <c r="A6" s="9" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>25</v>
@@ -2868,10 +2876,10 @@
         <v>28</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>29</v>
@@ -2911,7 +2919,7 @@
     </row>
     <row r="7" spans="1:21" ht="17" customHeight="1">
       <c r="A7" s="9" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>23</v>
@@ -2920,10 +2928,10 @@
         <v>28</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>29</v>
@@ -2963,7 +2971,7 @@
     </row>
     <row r="8" spans="1:21" ht="17" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>24</v>
@@ -2972,10 +2980,10 @@
         <v>28</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>29</v>
@@ -3015,7 +3023,7 @@
     </row>
     <row r="9" spans="1:21" ht="17" customHeight="1">
       <c r="A9" s="9" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>25</v>
@@ -3024,10 +3032,10 @@
         <v>28</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>29</v>
@@ -3067,7 +3075,7 @@
     </row>
     <row r="10" spans="1:21" ht="17" customHeight="1">
       <c r="A10" s="9" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>23</v>
@@ -3076,10 +3084,10 @@
         <v>28</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>209</v>
+        <v>250</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>29</v>
@@ -3119,7 +3127,7 @@
     </row>
     <row r="11" spans="1:21" ht="17" customHeight="1">
       <c r="A11" s="9" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>24</v>
@@ -3128,10 +3136,10 @@
         <v>28</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>209</v>
+        <v>250</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>29</v>
@@ -3171,7 +3179,7 @@
     </row>
     <row r="12" spans="1:21" ht="17" customHeight="1">
       <c r="A12" s="9" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>25</v>
@@ -3180,10 +3188,10 @@
         <v>28</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>209</v>
+        <v>250</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>29</v>
@@ -3223,7 +3231,7 @@
     </row>
     <row r="13" spans="1:21" ht="17" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>23</v>
@@ -3235,7 +3243,7 @@
         <v>143</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>29</v>
@@ -3275,7 +3283,7 @@
     </row>
     <row r="14" spans="1:21" ht="17" customHeight="1">
       <c r="A14" s="9" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>24</v>
@@ -3287,7 +3295,7 @@
         <v>143</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>29</v>
@@ -3327,7 +3335,7 @@
     </row>
     <row r="15" spans="1:21" ht="17" customHeight="1">
       <c r="A15" s="9" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>25</v>
@@ -3339,7 +3347,7 @@
         <v>143</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="F15" s="10" t="s">
         <v>29</v>
@@ -3379,7 +3387,7 @@
     </row>
     <row r="16" spans="1:21" ht="17" customHeight="1">
       <c r="A16" s="9" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>23</v>
@@ -3388,10 +3396,10 @@
         <v>28</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>209</v>
+        <v>250</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>29</v>
@@ -3431,7 +3439,7 @@
     </row>
     <row r="17" spans="1:20" ht="17" customHeight="1">
       <c r="A17" s="9" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>24</v>
@@ -3440,10 +3448,10 @@
         <v>28</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>209</v>
+        <v>250</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>29</v>
@@ -3483,7 +3491,7 @@
     </row>
     <row r="18" spans="1:20" ht="17" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>26</v>
@@ -3492,10 +3500,10 @@
         <v>28</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>209</v>
+        <v>250</v>
       </c>
       <c r="F18" s="10" t="s">
         <v>29</v>
@@ -3536,7 +3544,7 @@
     <row r="19" spans="1:20" s="14" customFormat="1" ht="17" customHeight="1"/>
     <row r="20" spans="1:20" ht="17" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>20</v>
@@ -3545,10 +3553,10 @@
         <v>2</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="F20" s="10" t="s">
         <v>8</v>
@@ -3588,7 +3596,7 @@
     </row>
     <row r="21" spans="1:20" ht="17" customHeight="1">
       <c r="A21" s="9" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>19</v>
@@ -3597,10 +3605,10 @@
         <v>2</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>8</v>
@@ -3640,7 +3648,7 @@
     </row>
     <row r="22" spans="1:20" ht="17" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>6</v>
@@ -3649,10 +3657,10 @@
         <v>2</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="F22" s="9" t="s">
         <v>61</v>
@@ -3692,7 +3700,7 @@
     </row>
     <row r="23" spans="1:20" ht="17" customHeight="1">
       <c r="A23" s="9" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>7</v>
@@ -3701,10 +3709,10 @@
         <v>2</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="F23" s="9" t="s">
         <v>61</v>
@@ -3745,7 +3753,7 @@
     <row r="24" spans="1:20" s="14" customFormat="1" ht="17" customHeight="1"/>
     <row r="25" spans="1:20" ht="17" customHeight="1">
       <c r="A25" s="9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>203</v>
@@ -3754,10 +3762,10 @@
         <v>41</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="F25" s="10" t="s">
         <v>60</v>
@@ -3795,7 +3803,7 @@
     </row>
     <row r="26" spans="1:20" ht="17" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>204</v>
@@ -3804,10 +3812,10 @@
         <v>42</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="F26" s="10" t="s">
         <v>60</v>
@@ -3828,7 +3836,7 @@
         <v>16</v>
       </c>
       <c r="L26" s="24" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="M26" s="12">
         <v>1</v>
@@ -3843,7 +3851,7 @@
     </row>
     <row r="27" spans="1:20" ht="17" customHeight="1">
       <c r="A27" s="9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>205</v>
@@ -3852,10 +3860,10 @@
         <v>43</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>44</v>
@@ -3897,7 +3905,7 @@
     </row>
     <row r="28" spans="1:20" ht="17" customHeight="1">
       <c r="A28" s="9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>206</v>
@@ -3906,10 +3914,10 @@
         <v>144</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>44</v>
@@ -3930,7 +3938,7 @@
         <v>16</v>
       </c>
       <c r="L28" s="24" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="M28" s="9">
         <v>21</v>
@@ -3951,7 +3959,7 @@
     </row>
     <row r="29" spans="1:20" ht="17" customHeight="1">
       <c r="A29" s="9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>207</v>
@@ -3960,10 +3968,10 @@
         <v>145</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="F29" s="9" t="s">
         <v>45</v>
@@ -4005,19 +4013,19 @@
     </row>
     <row r="30" spans="1:20" ht="17" customHeight="1">
       <c r="A30" s="9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>59</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="F30" s="10" t="s">
         <v>60</v>
@@ -4055,7 +4063,7 @@
     </row>
     <row r="31" spans="1:20" ht="17" customHeight="1">
       <c r="A31" s="9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>32</v>
@@ -4064,10 +4072,10 @@
         <v>62</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="F31" s="10" t="s">
         <v>60</v>
@@ -4105,19 +4113,19 @@
     </row>
     <row r="32" spans="1:20" ht="17" customHeight="1">
       <c r="A32" s="9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>63</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="F32" s="13" t="s">
         <v>70</v>
@@ -4157,19 +4165,19 @@
     </row>
     <row r="33" spans="1:20" ht="17" customHeight="1">
       <c r="A33" s="9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="C33" s="18" t="s">
         <v>69</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="F33" s="13" t="s">
         <v>70</v>
@@ -4211,7 +4219,7 @@
     </row>
     <row r="34" spans="1:20" ht="17" customHeight="1">
       <c r="A34" s="9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B34" s="10" t="s">
         <v>39</v>
@@ -4262,19 +4270,19 @@
     </row>
     <row r="35" spans="1:20" ht="17" customHeight="1">
       <c r="A35" s="9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>78</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="F35" s="19" t="s">
         <v>79</v>
@@ -4312,7 +4320,7 @@
     </row>
     <row r="36" spans="1:20" ht="17" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>80</v>
@@ -4321,10 +4329,10 @@
         <v>71</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="F36" s="13" t="s">
         <v>70</v>
@@ -4348,7 +4356,7 @@
         <v>171</v>
       </c>
       <c r="M36" s="18" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="N36" s="23">
         <v>42185</v>
@@ -4362,7 +4370,7 @@
     </row>
     <row r="37" spans="1:20" ht="17" customHeight="1">
       <c r="A37" s="9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>34</v>
@@ -4371,10 +4379,10 @@
         <v>81</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="F37" s="13" t="s">
         <v>70</v>
@@ -4398,7 +4406,7 @@
         <v>171</v>
       </c>
       <c r="M37" s="10" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="N37" s="23">
         <v>42277</v>
@@ -4412,7 +4420,7 @@
     </row>
     <row r="38" spans="1:20" ht="17" customHeight="1">
       <c r="A38" s="9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B38" s="9" t="s">
         <v>31</v>
@@ -4424,7 +4432,7 @@
         <v>56</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="F38" s="10" t="s">
         <v>57</v>
@@ -4466,7 +4474,7 @@
     </row>
     <row r="39" spans="1:20" ht="17" customHeight="1">
       <c r="A39" s="9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B39" s="9" t="s">
         <v>33</v>
@@ -4478,7 +4486,7 @@
         <v>82</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="F39" s="10" t="s">
         <v>97</v>
@@ -4521,7 +4529,7 @@
     </row>
     <row r="40" spans="1:20" ht="17" customHeight="1">
       <c r="A40" s="9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>35</v>
@@ -4533,7 +4541,7 @@
         <v>85</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="F40" s="19" t="s">
         <v>98</v>
@@ -4576,7 +4584,7 @@
     </row>
     <row r="41" spans="1:20" ht="17" customHeight="1">
       <c r="A41" s="9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B41" s="9" t="s">
         <v>36</v>
@@ -4585,10 +4593,10 @@
         <v>102</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="F41" s="10" t="s">
         <v>104</v>
@@ -4609,7 +4617,7 @@
         <v>16</v>
       </c>
       <c r="L41" s="24" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="M41" s="10" t="s">
         <v>73</v>
@@ -4626,7 +4634,7 @@
     </row>
     <row r="42" spans="1:20" ht="17" customHeight="1">
       <c r="A42" s="9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B42" s="9" t="s">
         <v>37</v>
@@ -4635,10 +4643,10 @@
         <v>147</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="F42" s="10" t="s">
         <v>104</v>
@@ -4676,7 +4684,7 @@
     </row>
     <row r="43" spans="1:20" ht="17" customHeight="1">
       <c r="A43" s="9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>38</v>
@@ -4685,10 +4693,10 @@
         <v>103</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="F43" s="10" t="s">
         <v>105</v>
@@ -4709,7 +4717,7 @@
         <v>16</v>
       </c>
       <c r="L43" s="24" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="M43" s="10" t="s">
         <v>73</v>
@@ -4725,7 +4733,7 @@
     </row>
     <row r="44" spans="1:20" ht="17" customHeight="1">
       <c r="A44" s="9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B44" s="10" t="s">
         <v>40</v>
@@ -4734,10 +4742,10 @@
         <v>111</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="F44" s="15" t="s">
         <v>22</v>
@@ -4775,7 +4783,7 @@
     <row r="45" spans="1:20" s="14" customFormat="1" ht="17" customHeight="1"/>
     <row r="46" spans="1:20" ht="17" customHeight="1">
       <c r="A46" s="10" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B46" s="10" t="s">
         <v>113</v>
@@ -4784,10 +4792,10 @@
         <v>115</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="F46" s="15" t="s">
         <v>118</v>
@@ -4828,7 +4836,7 @@
     </row>
     <row r="47" spans="1:20" ht="17" customHeight="1">
       <c r="A47" s="10" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B47" s="10" t="s">
         <v>114</v>
@@ -4837,10 +4845,10 @@
         <v>116</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="F47" s="15" t="s">
         <v>118</v>
@@ -4885,7 +4893,7 @@
     <row r="48" spans="1:20" s="14" customFormat="1" ht="17" customHeight="1"/>
     <row r="49" spans="1:17" ht="17" customHeight="1">
       <c r="A49" s="10" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B49" s="10" t="s">
         <v>121</v>
@@ -4894,10 +4902,10 @@
         <v>127</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>210</v>
+        <v>258</v>
       </c>
       <c r="F49" s="10" t="s">
         <v>131</v>
@@ -4936,7 +4944,7 @@
     </row>
     <row r="50" spans="1:17" ht="17" customHeight="1">
       <c r="A50" s="10" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B50" s="10" t="s">
         <v>122</v>
@@ -4945,10 +4953,10 @@
         <v>146</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>210</v>
+        <v>258</v>
       </c>
       <c r="F50" s="10" t="s">
         <v>149</v>
@@ -4987,7 +4995,7 @@
     </row>
     <row r="51" spans="1:17" ht="17" customHeight="1">
       <c r="A51" s="10" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B51" s="10" t="s">
         <v>123</v>
@@ -4996,10 +5004,10 @@
         <v>148</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>210</v>
+        <v>258</v>
       </c>
       <c r="F51" s="10" t="s">
         <v>150</v>
@@ -5038,7 +5046,7 @@
     </row>
     <row r="52" spans="1:17" ht="17" customHeight="1">
       <c r="A52" s="10" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B52" s="10" t="s">
         <v>124</v>
@@ -5050,7 +5058,7 @@
         <v>3</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>211</v>
+        <v>259</v>
       </c>
       <c r="F52" s="10" t="s">
         <v>131</v>
@@ -5089,7 +5097,7 @@
     </row>
     <row r="53" spans="1:17" ht="17" customHeight="1">
       <c r="A53" s="10" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B53" s="10" t="s">
         <v>125</v>
@@ -5098,10 +5106,10 @@
         <v>129</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>210</v>
+        <v>258</v>
       </c>
       <c r="F53" s="10" t="s">
         <v>131</v>
@@ -5140,7 +5148,7 @@
     </row>
     <row r="54" spans="1:17" ht="17" customHeight="1">
       <c r="A54" s="10" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B54" s="10" t="s">
         <v>126</v>
@@ -5149,7 +5157,7 @@
         <v>130</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E54" s="15" t="s">
         <v>22</v>
@@ -5191,7 +5199,7 @@
     </row>
     <row r="55" spans="1:17" ht="17" customHeight="1">
       <c r="A55" s="10" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B55" s="10" t="s">
         <v>152</v>
@@ -5200,10 +5208,10 @@
         <v>151</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>210</v>
+        <v>258</v>
       </c>
       <c r="F55" s="10" t="s">
         <v>131</v>
@@ -5240,7 +5248,7 @@
     </row>
     <row r="56" spans="1:17" ht="17" customHeight="1">
       <c r="A56" s="10" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B56" s="10" t="s">
         <v>156</v>
@@ -5249,10 +5257,10 @@
         <v>154</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>212</v>
+        <v>260</v>
       </c>
       <c r="F56" s="10" t="s">
         <v>131</v>
@@ -5291,7 +5299,7 @@
     </row>
     <row r="57" spans="1:17" ht="17" customHeight="1">
       <c r="A57" s="10" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B57" s="10" t="s">
         <v>157</v>
@@ -5300,10 +5308,10 @@
         <v>153</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>212</v>
+        <v>260</v>
       </c>
       <c r="F57" s="10" t="s">
         <v>131</v>
@@ -5342,7 +5350,7 @@
     </row>
     <row r="58" spans="1:17" ht="17" customHeight="1">
       <c r="A58" s="10" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B58" s="10" t="s">
         <v>155</v>
@@ -5351,10 +5359,10 @@
         <v>158</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>212</v>
+        <v>260</v>
       </c>
       <c r="F58" s="10" t="s">
         <v>162</v>
@@ -5393,19 +5401,19 @@
     </row>
     <row r="59" spans="1:17" ht="17" customHeight="1">
       <c r="A59" s="10" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C59" s="10" t="s">
         <v>159</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>210</v>
+        <v>258</v>
       </c>
       <c r="F59" s="10" t="s">
         <v>131</v>
@@ -5444,19 +5452,19 @@
     </row>
     <row r="60" spans="1:17" ht="17" customHeight="1">
       <c r="A60" s="10" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C60" s="10" t="s">
         <v>160</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>210</v>
+        <v>258</v>
       </c>
       <c r="F60" s="10" t="s">
         <v>131</v>
@@ -5495,19 +5503,19 @@
     </row>
     <row r="61" spans="1:17" ht="17" customHeight="1">
       <c r="A61" s="10" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C61" s="10" t="s">
         <v>161</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>210</v>
+        <v>258</v>
       </c>
       <c r="F61" s="10" t="s">
         <v>131</v>
@@ -5547,7 +5555,7 @@
     <row r="62" spans="1:17" s="14" customFormat="1" ht="17" customHeight="1"/>
     <row r="63" spans="1:17" ht="17" customHeight="1">
       <c r="A63" s="10" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B63" s="10" t="s">
         <v>141</v>
@@ -5556,10 +5564,10 @@
         <v>140</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="F63" s="10" t="s">
         <v>142</v>
@@ -5600,7 +5608,7 @@
     </row>
     <row r="64" spans="1:17" ht="17" customHeight="1">
       <c r="A64" s="10" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B64" s="10" t="s">
         <v>141</v>
@@ -5609,10 +5617,10 @@
         <v>140</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="F64" s="10" t="s">
         <v>142</v>

</xml_diff>

<commit_message>
Added links and phase columns
</commit_message>
<xml_diff>
--- a/milestones-consolidated.xlsx
+++ b/milestones-consolidated.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="271">
   <si>
     <t>center</t>
   </si>
@@ -814,6 +814,24 @@
   </si>
   <si>
     <t>PHASE ONE DATA COMING SOON</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/db/datasets/20215/</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/db/datasets/20216/</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/db/datasets/20217/</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/db/datasets/20218/</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/db/datasets/20219/</t>
+  </si>
+  <si>
+    <t>release-link</t>
   </si>
 </sst>
 </file>
@@ -995,7 +1013,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="649">
+  <cellStyleXfs count="651">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1645,8 +1663,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1706,8 +1726,9 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="649"/>
   </cellXfs>
-  <cellStyles count="649">
+  <cellStyles count="651">
     <cellStyle name="Bad" xfId="43" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2031,6 +2052,7 @@
     <cellStyle name="Followed Hyperlink" xfId="644" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="646" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="648" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="650" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2353,6 +2375,7 @@
     <cellStyle name="Hyperlink" xfId="643" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="645" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="647" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="649" builtinId="8"/>
     <cellStyle name="Neutral" xfId="377" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="140"/>
@@ -2693,10 +2716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U70"/>
+  <dimension ref="A1:V70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0"/>
@@ -2716,14 +2739,15 @@
     <col min="13" max="13" width="10.6640625" style="10" customWidth="1"/>
     <col min="14" max="14" width="16.33203125" style="10" bestFit="1" customWidth="1"/>
     <col min="15" max="17" width="15.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="50" style="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.6640625" style="10" customWidth="1"/>
-    <col min="20" max="20" width="104.83203125" style="10" customWidth="1"/>
-    <col min="21" max="21" width="5.6640625" style="10" customWidth="1"/>
-    <col min="22" max="16384" width="10.83203125" style="10"/>
+    <col min="18" max="18" width="15.33203125" style="10" customWidth="1"/>
+    <col min="19" max="19" width="50" style="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.6640625" style="10" customWidth="1"/>
+    <col min="21" max="21" width="104.83203125" style="10" customWidth="1"/>
+    <col min="22" max="22" width="5.6640625" style="10" customWidth="1"/>
+    <col min="23" max="16384" width="10.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="6" customFormat="1" ht="30">
+    <row r="1" spans="1:22" s="6" customFormat="1" ht="30">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2775,13 +2799,16 @@
       <c r="Q1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="S1" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="T1" s="5"/>
-      <c r="U1" s="2"/>
-    </row>
-    <row r="2" spans="1:21" s="6" customFormat="1" ht="17" customHeight="1">
+      <c r="U1" s="5"/>
+      <c r="V1" s="2"/>
+    </row>
+    <row r="2" spans="1:22" s="6" customFormat="1" ht="17" customHeight="1">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -2825,10 +2852,11 @@
       <c r="Q2" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="T2" s="5"/>
-      <c r="U2" s="2"/>
-    </row>
-    <row r="3" spans="1:21" s="8" customFormat="1" ht="17" customHeight="1">
+      <c r="R2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="2"/>
+    </row>
+    <row r="3" spans="1:22" s="8" customFormat="1" ht="17" customHeight="1">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -2844,10 +2872,10 @@
       </c>
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="3"/>
-    </row>
-    <row r="4" spans="1:21" ht="17" customHeight="1">
+      <c r="U3" s="7"/>
+      <c r="V3" s="3"/>
+    </row>
+    <row r="4" spans="1:22" ht="17" customHeight="1">
       <c r="A4" s="9" t="s">
         <v>237</v>
       </c>
@@ -2897,12 +2925,13 @@
       <c r="Q4" s="23">
         <v>42124</v>
       </c>
-      <c r="R4" s="10">
-        <v>2</v>
-      </c>
-      <c r="T4" s="9"/>
-    </row>
-    <row r="5" spans="1:21" ht="17" customHeight="1">
+      <c r="R4" s="23"/>
+      <c r="S4" s="10">
+        <v>2</v>
+      </c>
+      <c r="U4" s="9"/>
+    </row>
+    <row r="5" spans="1:22" ht="17" customHeight="1">
       <c r="A5" s="9" t="s">
         <v>237</v>
       </c>
@@ -2952,12 +2981,13 @@
       <c r="Q5" s="23">
         <v>42124</v>
       </c>
-      <c r="R5" s="10">
-        <v>2</v>
-      </c>
-      <c r="T5" s="9"/>
-    </row>
-    <row r="6" spans="1:21" ht="17" customHeight="1">
+      <c r="R5" s="23"/>
+      <c r="S5" s="10">
+        <v>2</v>
+      </c>
+      <c r="U5" s="9"/>
+    </row>
+    <row r="6" spans="1:22" ht="17" customHeight="1">
       <c r="A6" s="9" t="s">
         <v>237</v>
       </c>
@@ -3007,12 +3037,13 @@
       <c r="Q6" s="23">
         <v>42124</v>
       </c>
-      <c r="R6" s="10">
-        <v>2</v>
-      </c>
-      <c r="T6" s="9"/>
-    </row>
-    <row r="7" spans="1:21" ht="17" customHeight="1">
+      <c r="R6" s="23"/>
+      <c r="S6" s="10">
+        <v>2</v>
+      </c>
+      <c r="U6" s="9"/>
+    </row>
+    <row r="7" spans="1:22" ht="17" customHeight="1">
       <c r="A7" s="9" t="s">
         <v>237</v>
       </c>
@@ -3062,12 +3093,13 @@
       <c r="Q7" s="23">
         <v>42216</v>
       </c>
-      <c r="R7" s="10">
-        <v>2</v>
-      </c>
-      <c r="T7" s="1"/>
-    </row>
-    <row r="8" spans="1:21" ht="17" customHeight="1">
+      <c r="R7" s="23"/>
+      <c r="S7" s="10">
+        <v>2</v>
+      </c>
+      <c r="U7" s="1"/>
+    </row>
+    <row r="8" spans="1:22" ht="17" customHeight="1">
       <c r="A8" s="9" t="s">
         <v>237</v>
       </c>
@@ -3117,12 +3149,13 @@
       <c r="Q8" s="23">
         <v>42216</v>
       </c>
-      <c r="R8" s="10">
-        <v>2</v>
-      </c>
-      <c r="T8" s="1"/>
-    </row>
-    <row r="9" spans="1:21" ht="17" customHeight="1">
+      <c r="R8" s="23"/>
+      <c r="S8" s="10">
+        <v>2</v>
+      </c>
+      <c r="U8" s="1"/>
+    </row>
+    <row r="9" spans="1:22" ht="17" customHeight="1">
       <c r="A9" s="9" t="s">
         <v>237</v>
       </c>
@@ -3172,12 +3205,13 @@
       <c r="Q9" s="23">
         <v>42216</v>
       </c>
-      <c r="R9" s="10">
-        <v>2</v>
-      </c>
-      <c r="T9" s="1"/>
-    </row>
-    <row r="10" spans="1:21" ht="17" customHeight="1">
+      <c r="R9" s="23"/>
+      <c r="S9" s="10">
+        <v>2</v>
+      </c>
+      <c r="U9" s="1"/>
+    </row>
+    <row r="10" spans="1:22" ht="17" customHeight="1">
       <c r="A10" s="9" t="s">
         <v>237</v>
       </c>
@@ -3227,12 +3261,13 @@
       <c r="Q10" s="23">
         <v>42292</v>
       </c>
-      <c r="R10" s="10">
-        <v>2</v>
-      </c>
-      <c r="T10" s="1"/>
-    </row>
-    <row r="11" spans="1:21" ht="17" customHeight="1">
+      <c r="R10" s="23"/>
+      <c r="S10" s="10">
+        <v>2</v>
+      </c>
+      <c r="U10" s="1"/>
+    </row>
+    <row r="11" spans="1:22" ht="17" customHeight="1">
       <c r="A11" s="9" t="s">
         <v>237</v>
       </c>
@@ -3282,12 +3317,13 @@
       <c r="Q11" s="23">
         <v>42292</v>
       </c>
-      <c r="R11" s="10">
-        <v>2</v>
-      </c>
-      <c r="T11" s="1"/>
-    </row>
-    <row r="12" spans="1:21" ht="17" customHeight="1">
+      <c r="R11" s="23"/>
+      <c r="S11" s="10">
+        <v>2</v>
+      </c>
+      <c r="U11" s="1"/>
+    </row>
+    <row r="12" spans="1:22" ht="17" customHeight="1">
       <c r="A12" s="9" t="s">
         <v>237</v>
       </c>
@@ -3337,12 +3373,13 @@
       <c r="Q12" s="23">
         <v>42292</v>
       </c>
-      <c r="R12" s="10">
-        <v>2</v>
-      </c>
-      <c r="T12" s="1"/>
-    </row>
-    <row r="13" spans="1:21" ht="17" customHeight="1">
+      <c r="R12" s="23"/>
+      <c r="S12" s="10">
+        <v>2</v>
+      </c>
+      <c r="U12" s="1"/>
+    </row>
+    <row r="13" spans="1:22" ht="17" customHeight="1">
       <c r="A13" s="9" t="s">
         <v>237</v>
       </c>
@@ -3392,12 +3429,13 @@
       <c r="Q13" s="23">
         <v>42292</v>
       </c>
-      <c r="R13" s="10">
-        <v>2</v>
-      </c>
-      <c r="T13" s="1"/>
-    </row>
-    <row r="14" spans="1:21" ht="17" customHeight="1">
+      <c r="R13" s="23"/>
+      <c r="S13" s="10">
+        <v>2</v>
+      </c>
+      <c r="U13" s="1"/>
+    </row>
+    <row r="14" spans="1:22" ht="17" customHeight="1">
       <c r="A14" s="9" t="s">
         <v>237</v>
       </c>
@@ -3447,12 +3485,13 @@
       <c r="Q14" s="23">
         <v>42292</v>
       </c>
-      <c r="R14" s="10">
-        <v>2</v>
-      </c>
-      <c r="T14" s="1"/>
-    </row>
-    <row r="15" spans="1:21" ht="17" customHeight="1">
+      <c r="R14" s="23"/>
+      <c r="S14" s="10">
+        <v>2</v>
+      </c>
+      <c r="U14" s="1"/>
+    </row>
+    <row r="15" spans="1:22" ht="17" customHeight="1">
       <c r="A15" s="9" t="s">
         <v>237</v>
       </c>
@@ -3502,12 +3541,13 @@
       <c r="Q15" s="23">
         <v>42292</v>
       </c>
-      <c r="R15" s="10">
-        <v>2</v>
-      </c>
-      <c r="T15" s="1"/>
-    </row>
-    <row r="16" spans="1:21" ht="17" customHeight="1">
+      <c r="R15" s="23"/>
+      <c r="S15" s="10">
+        <v>2</v>
+      </c>
+      <c r="U15" s="1"/>
+    </row>
+    <row r="16" spans="1:22" ht="17" customHeight="1">
       <c r="A16" s="9" t="s">
         <v>237</v>
       </c>
@@ -3557,12 +3597,13 @@
       <c r="Q16" s="23">
         <v>42400</v>
       </c>
-      <c r="R16" s="10">
-        <v>2</v>
-      </c>
-      <c r="T16" s="1"/>
-    </row>
-    <row r="17" spans="1:20" ht="17" customHeight="1">
+      <c r="R16" s="23"/>
+      <c r="S16" s="10">
+        <v>2</v>
+      </c>
+      <c r="U16" s="1"/>
+    </row>
+    <row r="17" spans="1:21" ht="17" customHeight="1">
       <c r="A17" s="9" t="s">
         <v>237</v>
       </c>
@@ -3612,12 +3653,13 @@
       <c r="Q17" s="23">
         <v>42400</v>
       </c>
-      <c r="R17" s="10">
-        <v>2</v>
-      </c>
-      <c r="T17" s="1"/>
-    </row>
-    <row r="18" spans="1:20" ht="17" customHeight="1">
+      <c r="R17" s="23"/>
+      <c r="S17" s="10">
+        <v>2</v>
+      </c>
+      <c r="U17" s="1"/>
+    </row>
+    <row r="18" spans="1:21" ht="17" customHeight="1">
       <c r="A18" s="9" t="s">
         <v>237</v>
       </c>
@@ -3667,13 +3709,14 @@
       <c r="Q18" s="23">
         <v>42400</v>
       </c>
-      <c r="R18" s="10">
-        <v>2</v>
-      </c>
-      <c r="T18" s="1"/>
-    </row>
-    <row r="19" spans="1:20" s="14" customFormat="1" ht="17" customHeight="1"/>
-    <row r="20" spans="1:20" ht="17" customHeight="1">
+      <c r="R18" s="23"/>
+      <c r="S18" s="10">
+        <v>2</v>
+      </c>
+      <c r="U18" s="1"/>
+    </row>
+    <row r="19" spans="1:21" s="14" customFormat="1" ht="17" customHeight="1"/>
+    <row r="20" spans="1:21" ht="17" customHeight="1">
       <c r="A20" s="9" t="s">
         <v>207</v>
       </c>
@@ -3723,12 +3766,13 @@
       <c r="Q20" s="23">
         <v>42185</v>
       </c>
-      <c r="R20" s="4">
-        <v>2</v>
-      </c>
-      <c r="T20" s="9"/>
-    </row>
-    <row r="21" spans="1:20" ht="17" customHeight="1">
+      <c r="R20" s="23"/>
+      <c r="S20" s="4">
+        <v>2</v>
+      </c>
+      <c r="U20" s="9"/>
+    </row>
+    <row r="21" spans="1:21" ht="17" customHeight="1">
       <c r="A21" s="9" t="s">
         <v>207</v>
       </c>
@@ -3778,12 +3822,13 @@
       <c r="Q21" s="23">
         <v>42185</v>
       </c>
-      <c r="R21" s="4">
-        <v>2</v>
-      </c>
-      <c r="T21" s="9"/>
-    </row>
-    <row r="22" spans="1:20" ht="17" customHeight="1">
+      <c r="R21" s="23"/>
+      <c r="S21" s="4">
+        <v>2</v>
+      </c>
+      <c r="U21" s="9"/>
+    </row>
+    <row r="22" spans="1:21" ht="17" customHeight="1">
       <c r="A22" s="9" t="s">
         <v>207</v>
       </c>
@@ -3833,12 +3878,13 @@
       <c r="Q22" s="23">
         <v>42185</v>
       </c>
-      <c r="R22" s="4">
-        <v>2</v>
-      </c>
-      <c r="T22" s="9"/>
-    </row>
-    <row r="23" spans="1:20" ht="17" customHeight="1">
+      <c r="R22" s="23"/>
+      <c r="S22" s="4">
+        <v>2</v>
+      </c>
+      <c r="U22" s="9"/>
+    </row>
+    <row r="23" spans="1:21" ht="17" customHeight="1">
       <c r="A23" s="9" t="s">
         <v>207</v>
       </c>
@@ -3888,13 +3934,14 @@
       <c r="Q23" s="23">
         <v>42185</v>
       </c>
-      <c r="R23" s="4">
-        <v>2</v>
-      </c>
-      <c r="T23" s="9"/>
-    </row>
-    <row r="24" spans="1:20" s="14" customFormat="1" ht="17" customHeight="1"/>
-    <row r="25" spans="1:20" ht="17" customHeight="1">
+      <c r="R23" s="23"/>
+      <c r="S23" s="4">
+        <v>2</v>
+      </c>
+      <c r="U23" s="9"/>
+    </row>
+    <row r="24" spans="1:21" s="14" customFormat="1" ht="17" customHeight="1"/>
+    <row r="25" spans="1:21" ht="17" customHeight="1">
       <c r="A25" s="9" t="s">
         <v>208</v>
       </c>
@@ -3942,12 +3989,15 @@
       </c>
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
-      <c r="R25" s="4">
-        <v>2</v>
-      </c>
-      <c r="T25" s="9"/>
-    </row>
-    <row r="26" spans="1:20" ht="17" customHeight="1">
+      <c r="R25" s="29" t="s">
+        <v>265</v>
+      </c>
+      <c r="S25" s="4">
+        <v>2</v>
+      </c>
+      <c r="U25" s="9"/>
+    </row>
+    <row r="26" spans="1:21" ht="17" customHeight="1">
       <c r="A26" s="9" t="s">
         <v>208</v>
       </c>
@@ -3993,12 +4043,15 @@
         <v>42004</v>
       </c>
       <c r="Q26" s="4"/>
-      <c r="R26" s="4">
-        <v>2</v>
-      </c>
-      <c r="T26" s="9"/>
-    </row>
-    <row r="27" spans="1:20" ht="17" customHeight="1">
+      <c r="R26" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="S26" s="4">
+        <v>2</v>
+      </c>
+      <c r="U26" s="9"/>
+    </row>
+    <row r="27" spans="1:21" ht="17" customHeight="1">
       <c r="A27" s="9" t="s">
         <v>208</v>
       </c>
@@ -4050,12 +4103,15 @@
       <c r="Q27" s="23">
         <v>42094</v>
       </c>
-      <c r="R27" s="4">
-        <v>2</v>
-      </c>
-      <c r="T27" s="9"/>
-    </row>
-    <row r="28" spans="1:20" ht="17" customHeight="1">
+      <c r="R27" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="S27" s="4">
+        <v>2</v>
+      </c>
+      <c r="U27" s="9"/>
+    </row>
+    <row r="28" spans="1:21" ht="17" customHeight="1">
       <c r="A28" s="9" t="s">
         <v>208</v>
       </c>
@@ -4107,12 +4163,15 @@
       <c r="Q28" s="23">
         <v>42094</v>
       </c>
-      <c r="R28" s="4">
-        <v>2</v>
-      </c>
-      <c r="T28" s="9"/>
-    </row>
-    <row r="29" spans="1:20" ht="17" customHeight="1">
+      <c r="R28" s="29" t="s">
+        <v>268</v>
+      </c>
+      <c r="S28" s="4">
+        <v>2</v>
+      </c>
+      <c r="U28" s="9"/>
+    </row>
+    <row r="29" spans="1:21" ht="17" customHeight="1">
       <c r="A29" s="9" t="s">
         <v>208</v>
       </c>
@@ -4164,12 +4223,15 @@
       <c r="Q29" s="23">
         <v>42094</v>
       </c>
-      <c r="R29" s="4">
-        <v>2</v>
-      </c>
-      <c r="T29" s="9"/>
-    </row>
-    <row r="30" spans="1:20" ht="17" customHeight="1">
+      <c r="R29" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="S29" s="4">
+        <v>2</v>
+      </c>
+      <c r="U29" s="9"/>
+    </row>
+    <row r="30" spans="1:21" ht="17" customHeight="1">
       <c r="A30" s="9" t="s">
         <v>208</v>
       </c>
@@ -4217,12 +4279,13 @@
       </c>
       <c r="P30" s="4"/>
       <c r="Q30" s="4"/>
-      <c r="R30" s="4">
-        <v>2</v>
-      </c>
-      <c r="T30" s="9"/>
-    </row>
-    <row r="31" spans="1:20" ht="17" customHeight="1">
+      <c r="R30" s="4"/>
+      <c r="S30" s="4">
+        <v>2</v>
+      </c>
+      <c r="U30" s="9"/>
+    </row>
+    <row r="31" spans="1:21" ht="17" customHeight="1">
       <c r="A31" s="9" t="s">
         <v>208</v>
       </c>
@@ -4270,12 +4333,13 @@
       </c>
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
-      <c r="R31" s="4">
-        <v>2</v>
-      </c>
-      <c r="T31" s="9"/>
-    </row>
-    <row r="32" spans="1:20" ht="17" customHeight="1">
+      <c r="R31" s="4"/>
+      <c r="S31" s="4">
+        <v>2</v>
+      </c>
+      <c r="U31" s="9"/>
+    </row>
+    <row r="32" spans="1:21" ht="17" customHeight="1">
       <c r="A32" s="9" t="s">
         <v>208</v>
       </c>
@@ -4325,12 +4389,13 @@
       <c r="Q32" s="23">
         <v>42369</v>
       </c>
-      <c r="R32" s="4">
-        <v>2</v>
-      </c>
-      <c r="T32" s="9"/>
-    </row>
-    <row r="33" spans="1:20" ht="17" customHeight="1">
+      <c r="R32" s="23"/>
+      <c r="S32" s="4">
+        <v>2</v>
+      </c>
+      <c r="U32" s="9"/>
+    </row>
+    <row r="33" spans="1:21" ht="17" customHeight="1">
       <c r="A33" s="9" t="s">
         <v>208</v>
       </c>
@@ -4382,12 +4447,13 @@
       <c r="Q33" s="23">
         <v>42369</v>
       </c>
-      <c r="R33" s="4">
-        <v>2</v>
-      </c>
-      <c r="T33" s="9"/>
-    </row>
-    <row r="34" spans="1:20" ht="17" customHeight="1">
+      <c r="R33" s="23"/>
+      <c r="S33" s="4">
+        <v>2</v>
+      </c>
+      <c r="U33" s="9"/>
+    </row>
+    <row r="34" spans="1:21" ht="17" customHeight="1">
       <c r="A34" s="9" t="s">
         <v>208</v>
       </c>
@@ -4437,11 +4503,12 @@
         <v>42369</v>
       </c>
       <c r="Q34" s="4"/>
-      <c r="R34" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" ht="17" customHeight="1">
+      <c r="R34" s="4"/>
+      <c r="S34" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" ht="17" customHeight="1">
       <c r="A35" s="9" t="s">
         <v>208</v>
       </c>
@@ -4489,12 +4556,13 @@
       </c>
       <c r="P35" s="4"/>
       <c r="Q35" s="4"/>
-      <c r="R35" s="4">
-        <v>2</v>
-      </c>
-      <c r="T35" s="9"/>
-    </row>
-    <row r="36" spans="1:20" ht="17" customHeight="1">
+      <c r="R35" s="4"/>
+      <c r="S35" s="4">
+        <v>2</v>
+      </c>
+      <c r="U35" s="9"/>
+    </row>
+    <row r="36" spans="1:21" ht="17" customHeight="1">
       <c r="A36" s="9" t="s">
         <v>208</v>
       </c>
@@ -4542,12 +4610,13 @@
       </c>
       <c r="P36" s="4"/>
       <c r="Q36" s="4"/>
-      <c r="R36" s="4">
-        <v>2</v>
-      </c>
-      <c r="T36" s="9"/>
-    </row>
-    <row r="37" spans="1:20" ht="17" customHeight="1">
+      <c r="R36" s="4"/>
+      <c r="S36" s="4">
+        <v>2</v>
+      </c>
+      <c r="U36" s="9"/>
+    </row>
+    <row r="37" spans="1:21" ht="17" customHeight="1">
       <c r="A37" s="9" t="s">
         <v>208</v>
       </c>
@@ -4595,12 +4664,13 @@
       </c>
       <c r="P37" s="4"/>
       <c r="Q37" s="4"/>
-      <c r="R37" s="4">
-        <v>2</v>
-      </c>
-      <c r="T37" s="9"/>
-    </row>
-    <row r="38" spans="1:20" ht="17" customHeight="1">
+      <c r="R37" s="4"/>
+      <c r="S37" s="4">
+        <v>2</v>
+      </c>
+      <c r="U37" s="9"/>
+    </row>
+    <row r="38" spans="1:21" ht="17" customHeight="1">
       <c r="A38" s="9" t="s">
         <v>208</v>
       </c>
@@ -4652,12 +4722,13 @@
       <c r="Q38" s="23">
         <v>42369</v>
       </c>
-      <c r="R38" s="4">
-        <v>2</v>
-      </c>
-      <c r="T38" s="9"/>
-    </row>
-    <row r="39" spans="1:20" ht="17" customHeight="1">
+      <c r="R38" s="23"/>
+      <c r="S38" s="4">
+        <v>2</v>
+      </c>
+      <c r="U38" s="9"/>
+    </row>
+    <row r="39" spans="1:21" ht="17" customHeight="1">
       <c r="A39" s="9" t="s">
         <v>208</v>
       </c>
@@ -4709,12 +4780,13 @@
       <c r="Q39" s="23">
         <v>42460</v>
       </c>
-      <c r="R39" s="4">
-        <v>2</v>
-      </c>
-      <c r="T39" s="9"/>
-    </row>
-    <row r="40" spans="1:20" ht="17" customHeight="1">
+      <c r="R39" s="23"/>
+      <c r="S39" s="4">
+        <v>2</v>
+      </c>
+      <c r="U39" s="9"/>
+    </row>
+    <row r="40" spans="1:21" ht="17" customHeight="1">
       <c r="A40" s="9" t="s">
         <v>208</v>
       </c>
@@ -4766,12 +4838,13 @@
       <c r="Q40" s="23">
         <v>42551</v>
       </c>
-      <c r="R40" s="4">
-        <v>2</v>
-      </c>
-      <c r="T40" s="9"/>
-    </row>
-    <row r="41" spans="1:20" ht="17" customHeight="1">
+      <c r="R40" s="23"/>
+      <c r="S40" s="4">
+        <v>2</v>
+      </c>
+      <c r="U40" s="9"/>
+    </row>
+    <row r="41" spans="1:21" ht="17" customHeight="1">
       <c r="A41" s="9" t="s">
         <v>208</v>
       </c>
@@ -4819,12 +4892,13 @@
       </c>
       <c r="P41" s="4"/>
       <c r="Q41" s="4"/>
-      <c r="R41" s="4">
-        <v>2</v>
-      </c>
-      <c r="T41" s="9"/>
-    </row>
-    <row r="42" spans="1:20" ht="17" customHeight="1">
+      <c r="R41" s="4"/>
+      <c r="S41" s="4">
+        <v>2</v>
+      </c>
+      <c r="U41" s="9"/>
+    </row>
+    <row r="42" spans="1:21" ht="17" customHeight="1">
       <c r="A42" s="9" t="s">
         <v>208</v>
       </c>
@@ -4872,12 +4946,13 @@
       </c>
       <c r="P42" s="4"/>
       <c r="Q42" s="4"/>
-      <c r="R42" s="4">
-        <v>2</v>
-      </c>
-      <c r="T42" s="9"/>
-    </row>
-    <row r="43" spans="1:20" ht="17" customHeight="1">
+      <c r="R42" s="4"/>
+      <c r="S42" s="4">
+        <v>2</v>
+      </c>
+      <c r="U42" s="9"/>
+    </row>
+    <row r="43" spans="1:21" ht="17" customHeight="1">
       <c r="A43" s="9" t="s">
         <v>208</v>
       </c>
@@ -4925,11 +5000,12 @@
       </c>
       <c r="P43" s="4"/>
       <c r="Q43" s="4"/>
-      <c r="R43" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" ht="17" customHeight="1">
+      <c r="R43" s="4"/>
+      <c r="S43" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" ht="17" customHeight="1">
       <c r="A44" s="9" t="s">
         <v>208</v>
       </c>
@@ -4977,12 +5053,13 @@
       </c>
       <c r="P44" s="4"/>
       <c r="Q44" s="4"/>
-      <c r="R44" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:20" s="14" customFormat="1" ht="17" customHeight="1"/>
-    <row r="46" spans="1:20" ht="17" customHeight="1">
+      <c r="R44" s="4"/>
+      <c r="S44" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" s="14" customFormat="1" ht="17" customHeight="1"/>
+    <row r="46" spans="1:21" ht="17" customHeight="1">
       <c r="A46" s="10" t="s">
         <v>210</v>
       </c>
@@ -5034,11 +5111,12 @@
       <c r="Q46" s="23">
         <v>42185</v>
       </c>
-      <c r="R46" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:20" ht="17" customHeight="1">
+      <c r="R46" s="23"/>
+      <c r="S46" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" ht="17" customHeight="1">
       <c r="A47" s="10" t="s">
         <v>210</v>
       </c>
@@ -5090,15 +5168,16 @@
       <c r="Q47" s="23">
         <v>42185</v>
       </c>
-      <c r="R47" s="4">
-        <v>2</v>
-      </c>
-      <c r="T47" s="19" t="s">
+      <c r="R47" s="23"/>
+      <c r="S47" s="4">
+        <v>2</v>
+      </c>
+      <c r="U47" s="19" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="48" spans="1:20" s="14" customFormat="1" ht="17" customHeight="1"/>
-    <row r="49" spans="1:18" ht="17" customHeight="1">
+    <row r="48" spans="1:21" s="14" customFormat="1" ht="17" customHeight="1"/>
+    <row r="49" spans="1:19" ht="17" customHeight="1">
       <c r="A49" s="10" t="s">
         <v>211</v>
       </c>
@@ -5148,11 +5227,12 @@
         <v>42369</v>
       </c>
       <c r="Q49" s="4"/>
-      <c r="R49" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" ht="17" customHeight="1">
+      <c r="R49" s="4"/>
+      <c r="S49" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" ht="17" customHeight="1">
       <c r="A50" s="10" t="s">
         <v>211</v>
       </c>
@@ -5202,11 +5282,12 @@
         <v>42369</v>
       </c>
       <c r="Q50" s="4"/>
-      <c r="R50" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" ht="17" customHeight="1">
+      <c r="R50" s="4"/>
+      <c r="S50" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" ht="17" customHeight="1">
       <c r="A51" s="10" t="s">
         <v>211</v>
       </c>
@@ -5256,11 +5337,12 @@
         <v>42369</v>
       </c>
       <c r="Q51" s="4"/>
-      <c r="R51" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" ht="17" customHeight="1">
+      <c r="R51" s="4"/>
+      <c r="S51" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" ht="17" customHeight="1">
       <c r="A52" s="10" t="s">
         <v>211</v>
       </c>
@@ -5310,11 +5392,12 @@
         <v>42369</v>
       </c>
       <c r="Q52" s="4"/>
-      <c r="R52" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:18" ht="17" customHeight="1">
+      <c r="R52" s="4"/>
+      <c r="S52" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" ht="17" customHeight="1">
       <c r="A53" s="10" t="s">
         <v>211</v>
       </c>
@@ -5364,11 +5447,12 @@
         <v>42369</v>
       </c>
       <c r="Q53" s="4"/>
-      <c r="R53" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18" ht="17" customHeight="1">
+      <c r="R53" s="4"/>
+      <c r="S53" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" ht="17" customHeight="1">
       <c r="A54" s="10" t="s">
         <v>211</v>
       </c>
@@ -5418,11 +5502,12 @@
         <v>42369</v>
       </c>
       <c r="Q54" s="4"/>
-      <c r="R54" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18" ht="17" customHeight="1">
+      <c r="R54" s="4"/>
+      <c r="S54" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" ht="17" customHeight="1">
       <c r="A55" s="10" t="s">
         <v>211</v>
       </c>
@@ -5470,11 +5555,12 @@
       </c>
       <c r="P55" s="4"/>
       <c r="Q55" s="4"/>
-      <c r="R55" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" ht="17" customHeight="1">
+      <c r="R55" s="4"/>
+      <c r="S55" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" ht="17" customHeight="1">
       <c r="A56" s="10" t="s">
         <v>211</v>
       </c>
@@ -5524,11 +5610,12 @@
         <v>42369</v>
       </c>
       <c r="Q56" s="4"/>
-      <c r="R56" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18" ht="17" customHeight="1">
+      <c r="R56" s="4"/>
+      <c r="S56" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" ht="17" customHeight="1">
       <c r="A57" s="10" t="s">
         <v>211</v>
       </c>
@@ -5578,11 +5665,12 @@
         <v>42369</v>
       </c>
       <c r="Q57" s="4"/>
-      <c r="R57" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" ht="17" customHeight="1">
+      <c r="R57" s="4"/>
+      <c r="S57" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" ht="17" customHeight="1">
       <c r="A58" s="10" t="s">
         <v>211</v>
       </c>
@@ -5632,11 +5720,12 @@
         <v>42369</v>
       </c>
       <c r="Q58" s="4"/>
-      <c r="R58" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:18" ht="17" customHeight="1">
+      <c r="R58" s="4"/>
+      <c r="S58" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" ht="17" customHeight="1">
       <c r="A59" s="10" t="s">
         <v>211</v>
       </c>
@@ -5686,11 +5775,12 @@
         <v>42369</v>
       </c>
       <c r="Q59" s="4"/>
-      <c r="R59" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:18" ht="17" customHeight="1">
+      <c r="R59" s="4"/>
+      <c r="S59" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" ht="17" customHeight="1">
       <c r="A60" s="10" t="s">
         <v>211</v>
       </c>
@@ -5740,11 +5830,12 @@
         <v>42369</v>
       </c>
       <c r="Q60" s="4"/>
-      <c r="R60" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:18" ht="17" customHeight="1">
+      <c r="R60" s="4"/>
+      <c r="S60" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" ht="17" customHeight="1">
       <c r="A61" s="10" t="s">
         <v>211</v>
       </c>
@@ -5794,12 +5885,13 @@
         <v>42369</v>
       </c>
       <c r="Q61" s="4"/>
-      <c r="R61" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:18" s="14" customFormat="1" ht="17" customHeight="1"/>
-    <row r="63" spans="1:18" ht="17" customHeight="1">
+      <c r="R61" s="4"/>
+      <c r="S61" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" s="14" customFormat="1" ht="17" customHeight="1"/>
+    <row r="63" spans="1:19" ht="17" customHeight="1">
       <c r="A63" s="10" t="s">
         <v>215</v>
       </c>
@@ -5851,11 +5943,12 @@
       <c r="Q63" s="23">
         <v>42277</v>
       </c>
-      <c r="R63" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" ht="17" customHeight="1">
+      <c r="R63" s="23"/>
+      <c r="S63" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" ht="17" customHeight="1">
       <c r="A64" s="10" t="s">
         <v>215</v>
       </c>
@@ -5907,11 +6000,12 @@
       <c r="Q64" s="23">
         <v>42459</v>
       </c>
-      <c r="R64" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:21" s="25" customFormat="1" ht="17" customHeight="1">
+      <c r="R64" s="23"/>
+      <c r="S64" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" s="25" customFormat="1" ht="17" customHeight="1">
       <c r="A65" s="26" t="s">
         <v>264</v>
       </c>
@@ -5934,33 +6028,34 @@
       <c r="R65" s="27"/>
       <c r="S65" s="27"/>
       <c r="T65" s="27"/>
-      <c r="U65" s="28"/>
-    </row>
-    <row r="66" spans="1:21" ht="17" customHeight="1">
+      <c r="U65" s="27"/>
+      <c r="V65" s="28"/>
+    </row>
+    <row r="66" spans="1:22" ht="17" customHeight="1">
       <c r="L66" s="4"/>
       <c r="M66" s="4"/>
       <c r="N66" s="4"/>
       <c r="O66" s="4"/>
     </row>
-    <row r="67" spans="1:21" ht="17" customHeight="1">
+    <row r="67" spans="1:22" ht="17" customHeight="1">
       <c r="L67" s="4"/>
       <c r="M67" s="4"/>
       <c r="N67" s="4"/>
       <c r="O67" s="4"/>
     </row>
-    <row r="68" spans="1:21" ht="17" customHeight="1">
+    <row r="68" spans="1:22" ht="17" customHeight="1">
       <c r="L68" s="4"/>
       <c r="M68" s="4"/>
       <c r="N68" s="4"/>
       <c r="O68" s="4"/>
     </row>
-    <row r="69" spans="1:21" ht="17" customHeight="1">
+    <row r="69" spans="1:22" ht="17" customHeight="1">
       <c r="L69" s="4"/>
       <c r="M69" s="4"/>
       <c r="N69" s="4"/>
       <c r="O69" s="4"/>
     </row>
-    <row r="70" spans="1:21" ht="17" customHeight="1">
+    <row r="70" spans="1:22" ht="17" customHeight="1">
       <c r="L70" s="4"/>
       <c r="M70" s="4"/>
       <c r="N70" s="4"/>
@@ -5968,8 +6063,15 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A65:U65"/>
+    <mergeCell ref="A65:V65"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="R28" r:id="rId1"/>
+    <hyperlink ref="R29" r:id="rId2"/>
+    <hyperlink ref="R27" r:id="rId3"/>
+    <hyperlink ref="R25" r:id="rId4"/>
+    <hyperlink ref="R26" r:id="rId5"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Updates to HMS Parsers
</commit_message>
<xml_diff>
--- a/milestones-consolidated.xlsx
+++ b/milestones-consolidated.xlsx
@@ -267,9 +267,6 @@
     <t>Human fibroblast-like synoviocytes lot #2586,Human fibroblast-like synoviocytes lot #2645,Human fibroblast-like synoviocytes lot #2759,Human fibroblast-like synoviocytes-RA lot #1869,Human fibroblast-like synoviocytes-RA lot 1931,Human fibroblast-like synoviocytes-RA lot #2159,Human fibroblast-like synoviocytes-RA lot #2708</t>
   </si>
   <si>
-    <t xml:space="preserve">Bead-based sandwich immunoassays--To generate measures of the secretion response landscape of seven primary human synovial fibroblast donors samples to stimulation with three stimuli in the presence or absence ot targeted inhibitors, with a key goal of evaluating variability of secretion response across patient samples. Supernatant levels of 51 cytokines, chemokines, growth factors, proteases, etc, are quantified. Indepedent experimental replicates are collected on separate days. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Bead-based sandwich immunoassays--To generate measures of (1) composition of synovial fluids from three RA patients, (2) to quantify secretion response of one primary human synovial fibroblast donor sample following individual exposure to synovial fluids from three RA patients, and (3) to quantify how this secretion response is altered by inhibition of MAP3K7/TAK1 by 5z-7-oxozeaenol. </t>
   </si>
   <si>
@@ -399,15 +396,9 @@
     <t>Imaging assay--monitoring cell survival in control, ALS, and SMA iMNs. iMNs will be transfected with a fluorescence reporter and imaged daily for 10 days. Images will be run through a custom analysis software package that tracks individual cells over time. The time of death (if it occurs) for each neuron will be determined. Neurite arborization will be determined using custom software analysis on these images. .</t>
   </si>
   <si>
-    <t>Baseline gene expression dataset for QC and pipeline development -- 11 total control iPSC cell lines 3 in triplicate and 1 in duplicate and 28 diseased iPSC, 4 ALS and 4 SMA with replicates and with no additional perturbagen. Determine cell line variability and assay reproducibility. RNAseq QC statistics and expression correlation statistics will guide the development of QC statndards and appropriate analysis pipeline.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Baseline gene expression dataset for iMN and diseased state signature -- 4 control, 4 ALS, and 4 SMA iPSC-derived iMN with replicates and with no additional perturbagen. Generate gene expression signatures and analyze disease/control contrast for statistically significant differentially expressed genes. Generate disease signatures for future systems analysis: pathway, network, and category enrichment analysis, as well as for integration with other omics and machine learning analyses. </t>
   </si>
   <si>
-    <t xml:space="preserve">Gene expression dataset for iMN and disease signature reponse to perturbagens -- 4 control, 4 ALS, and 4 SMA iPSC-derived iMN with replicates plus additional perturbagen. Generate gene expression signatures and for both disease and control and analyze perturb/disease &amp; perturb/control contrasts for statistically significant differentially expressed genes. Using a GLM setup multi-factor design matrix to analyze disease vs control with each perturbagen as an additional factor. Generate signatures for future systems analysis: pathway, network, and category enrichment analysis, as well as for integration with other omics and machine learning analyses. </t>
-  </si>
-  <si>
     <t>spinal muscular atrophy,disease;amyotrophic lateral sclerosis,disease</t>
   </si>
   <si>
@@ -435,9 +426,6 @@
     <t>spinal muscular atrophy,disease;amyotrophic lateral sclerosis,disease;TBD,small molecule</t>
   </si>
   <si>
-    <t>Use microenvironment microarray (MEMA) based platform to assess the impacts of ~3000 different pairwise combinations of ME perturbagens (MEPs) on 10 biological response endopoints.</t>
-  </si>
-  <si>
     <t>High-throughput MEMA array</t>
   </si>
   <si>
@@ -465,39 +453,18 @@
     <t>spinal muscular atrophy,disease;amyotrophic lateral sclerosis,disease;tunicamycin,small molecule</t>
   </si>
   <si>
-    <t>MS analysis on the QE and or Triple TOF MS instrument  of trypsin digested  iPSC dervied from 4 control, 4 ALS and 4 SMA lines for 3 different wells at  multiple cell passages.</t>
-  </si>
-  <si>
     <t>QC and SOP development for proteomic analysis  iPSC to  motor neuron differentiation</t>
   </si>
   <si>
-    <t>Build MS SWATH data library: using  the 6600 MS instrument analyzing either fractionated individuals and  pools of iPSC dervied from  4 controls and SMA and ALS lines into soluble, insoluble and acid soluble enriched for phosphorylation.</t>
-  </si>
-  <si>
-    <t>Build MS SWATH data library: using  the QE and 6600 MS instrument analyzing either fractionated individuals and pools of iPSC dervied from  4 controls and SMA and ALS lines into soluble, insoluble and acid soluble.</t>
-  </si>
-  <si>
     <t>Quantitative discovery proteomics (SWATH), add perturbagens</t>
   </si>
   <si>
-    <t>Quantitative discovery proteomics (SWATH), compare iPSC and mature differentitated neurons</t>
-  </si>
-  <si>
-    <t>Quantitative discovery proteomics (SWATH), compare iPSC, neural rosettes and differentated neurons</t>
-  </si>
-  <si>
     <t>Various perturbations on IPSC and potentially neurons. Analyze total protein and phosphorylation initially</t>
   </si>
   <si>
     <t>Baseline ATAC-seq experiments for protocol assay optimization, QC and development of analysis methods -- 4 control, 4 ALS and 4 SMA iPSC cell lines with replicates, without additional perturbagens. Determine optimal conditions for purification of high quality nuclei to preserve chromatin structure and for transposase reaction (number of nuclei, enzyme concentration and incubation time) to avoid over- or under-digestion. Set up analysis pipelines and perform correlation and clustering tests to determine cell line variability and assay reproducibility  between either technical or biological replicates and Identify potential problematic samples.</t>
   </si>
   <si>
-    <t>Baseline ATAC-seq experiments for iMN and disease state signatures -- 4 control, 4 ALS, and 4 SMA iPSC-derived iMN lines with replicates without additional perturbagens. Annotate open chromatin regions and map transcription factor binding events in regulatory elements genome-wide. Generate chromatin accessibility signatures  for each sample individually by calculating the enrichment of genomic regions relative to a set of control reads from Tn5-treated naked genomic DNA. Detect differential peaks between disease and control state. Generate disease signatures for future systems analysis and integration with other omics by 1) identifying genes mapping near differential peaks and detecting significantly enriched GO terms for these gene lists; 2) performing DNA foorprinting, motif scoring and applying regression methods to infer transcription factors responsible for gene expression signatures.</t>
-  </si>
-  <si>
-    <t>ATAC-seq dataset for iMN and disease signature reponse to perturbagens -- 4 control, 4 ALS, and 4 SMA iPSC-derived iMN lines with replicates plus additional perturbagens. Generate chromatin accessibility signatures  for each sample individually by calculating the enrichment of genomic regions relative to a set of control reads from Tn5-treated naked genomic DNA. Analyze perturb/disease &amp; perturb/control datasets to detecte differentially enriched peaks reflecting changes in chromatin structures as a consequence of perturbation. Generate disease signatures for future systems analysis and integration with other omics and machine learning analyses.</t>
-  </si>
-  <si>
     <t>spinal muscular atrophy,disease;amyotrophic lateral sclerosis,disease;stimulation A-N,stimulation</t>
   </si>
   <si>
@@ -832,6 +799,39 @@
   </si>
   <si>
     <t>phase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bead-based sandwich immunoassays--To generate measures of the secretion response landscape of seven primary human synovial fibroblast donors samples to stimulation with three stimuli in the presence or absence ot targeted inhibitors, with a key goal of evaluating variability of secretion response across patient samples. Supernatant levels of 51 cytokines, chemokines, growth factors, proteases, etc, are quantified. Independent experimental replicates are collected on separate days. </t>
+  </si>
+  <si>
+    <t>Baseline gene expression dataset for QC and pipeline development -- 11 total control iPSC cell lines 3 in triplicate and 1 in duplicate and 28 diseased iPSC, 4 ALS and 4 SMA with replicates and with no additional perturbagen. Determine cell line variability and assay reproducibility. RNAseq QC statistics and expression correlation statistics will guide the development of QC standards and appropriate analysis pipeline.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gene expression dataset for iMN and disease signature response to perturbagens -- 4 control, 4 ALS, and 4 SMA iPSC-derived iMN with replicates plus additional perturbagen. Generate gene expression signatures and for both disease and control and analyze perturb/disease &amp; perturb/control contrasts for statistically significant differentially expressed genes. Using a GLM setup multi-factor design matrix to analyze disease vs control with each perturbagen as an additional factor. Generate signatures for future systems analysis: pathway, network, and category enrichment analysis, as well as for integration with other omics and machine learning analyses. </t>
+  </si>
+  <si>
+    <t>MS analysis on the QE and or Triple TOF MS instrument  of trypsin digested  iPSC derived from 4 control, 4 ALS and 4 SMA lines for 3 different wells at  multiple cell passages.</t>
+  </si>
+  <si>
+    <t>Quantitative discovery proteomics (SWATH), compare iPSC and mature differentiated neurons</t>
+  </si>
+  <si>
+    <t>Build MS SWATH data library: using  the QE and 6600 MS instrument analyzing either fractionated individuals and pools of iPSC derived from  4 controls and SMA and ALS lines into soluble, insoluble and acid soluble.</t>
+  </si>
+  <si>
+    <t>Quantitative discovery proteomics (SWATH), compare iPSC, neural rosettes and differentiated neurons</t>
+  </si>
+  <si>
+    <t>Build MS SWATH data library: using  the 6600 MS instrument analyzing either fractionated individuals and  pools of iPSC derived from  4 controls and SMA and ALS lines into soluble, insoluble and acid soluble enriched for phosphorylation.</t>
+  </si>
+  <si>
+    <t>Baseline ATAC-seq experiments for iMN and disease state signatures -- 4 control, 4 ALS, and 4 SMA iPSC-derived iMN lines with replicates without additional perturbagens. Annotate open chromatin regions and map transcription factor binding events in regulatory elements genome-wide. Generate chromatin accessibility signatures  for each sample individually by calculating the enrichment of genomic regions relative to a set of control reads from Tn5-treated naked genomic DNA. Detect differential peaks between disease and control state. Generate disease signatures for future systems analysis and integration with other omics by 1) identifying genes mapping near differential peaks and detecting significantly enriched GO terms for these gene lists; 2) performing DNA foo printing, motif scoring and applying regression methods to infer transcription factors responsible for gene expression signatures.</t>
+  </si>
+  <si>
+    <t>ATAC-seq dataset for iMN and disease signature response to perturbagens -- 4 control, 4 ALS, and 4 SMA iPSC-derived iMN lines with replicates plus additional perturbagens. Generate chromatin accessibility signatures  for each sample individually by calculating the enrichment of genomic regions relative to a set of control reads from Tn5-treated naked genomic DNA. Analyze perturb/disease &amp; perturb/control datasets to detected differentially enriched peaks reflecting changes in chromatin structures as a consequence of perturbation. Generate disease signatures for future systems analysis and integration with other omics and machine learning analyses.</t>
+  </si>
+  <si>
+    <t>Use microenvironment microarray (MEMA) based platform to assess the impacts of ~3000 different pairwise combinations of ME perturbagens (MEPs) on 10 biological response endpoints.</t>
   </si>
 </sst>
 </file>
@@ -1009,7 +1009,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="658">
+  <cellStyleXfs count="659">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1660,6 +1660,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1738,7 +1739,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="658">
+  <cellStyles count="659">
     <cellStyle name="Bad" xfId="43" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2070,6 +2071,7 @@
     <cellStyle name="Followed Hyperlink" xfId="655" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="656" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="657" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="658" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2735,8 +2737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:T1048576"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0"/>
@@ -2787,7 +2789,7 @@
         <v>17</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>45</v>
@@ -2817,31 +2819,31 @@
         <v>1</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="S1" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>270</v>
       </c>
       <c r="V1" s="10"/>
     </row>
     <row r="2" spans="1:22" s="2" customFormat="1" ht="17" customHeight="1">
       <c r="D2" s="2" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>46</v>
@@ -2853,7 +2855,7 @@
         <v>15</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>64</v>
@@ -2868,19 +2870,19 @@
         <v>67</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="V2" s="10"/>
     </row>
     <row r="3" spans="1:22" s="2" customFormat="1" ht="17" customHeight="1">
       <c r="K3" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="V3" s="10"/>
     </row>
     <row r="4" spans="1:22" ht="17" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>23</v>
@@ -2889,19 +2891,19 @@
         <v>28</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>29</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>47</v>
@@ -2913,7 +2915,7 @@
         <v>16</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="M4" s="5"/>
       <c r="N4" s="11">
@@ -2935,7 +2937,7 @@
     </row>
     <row r="5" spans="1:22" ht="17" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>24</v>
@@ -2944,19 +2946,19 @@
         <v>28</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>29</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>47</v>
@@ -2968,7 +2970,7 @@
         <v>16</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="M5" s="5"/>
       <c r="N5" s="11">
@@ -2990,7 +2992,7 @@
     </row>
     <row r="6" spans="1:22" ht="17" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>25</v>
@@ -2999,19 +3001,19 @@
         <v>28</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>29</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>47</v>
@@ -3023,7 +3025,7 @@
         <v>16</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="M6" s="5"/>
       <c r="N6" s="11">
@@ -3045,7 +3047,7 @@
     </row>
     <row r="7" spans="1:22" ht="17" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>23</v>
@@ -3054,19 +3056,19 @@
         <v>28</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>29</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>47</v>
@@ -3078,7 +3080,7 @@
         <v>16</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="M7" s="5"/>
       <c r="N7" s="11">
@@ -3101,7 +3103,7 @@
     </row>
     <row r="8" spans="1:22" ht="17" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>24</v>
@@ -3110,19 +3112,19 @@
         <v>28</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>29</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>47</v>
@@ -3134,7 +3136,7 @@
         <v>16</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="M8" s="5"/>
       <c r="N8" s="11">
@@ -3157,7 +3159,7 @@
     </row>
     <row r="9" spans="1:22" ht="17" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>25</v>
@@ -3166,16 +3168,16 @@
         <v>28</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>29</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>47</v>
@@ -3187,7 +3189,7 @@
         <v>16</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="L9" s="5"/>
       <c r="M9" s="11">
@@ -3210,7 +3212,7 @@
     </row>
     <row r="10" spans="1:22" ht="17" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>23</v>
@@ -3219,16 +3221,16 @@
         <v>28</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>29</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>47</v>
@@ -3240,7 +3242,7 @@
         <v>16</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="L10" s="5"/>
       <c r="M10" s="11">
@@ -3263,7 +3265,7 @@
     </row>
     <row r="11" spans="1:22" ht="17" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>24</v>
@@ -3272,16 +3274,16 @@
         <v>28</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>29</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>47</v>
@@ -3293,7 +3295,7 @@
         <v>16</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="11">
@@ -3316,7 +3318,7 @@
     </row>
     <row r="12" spans="1:22" ht="17" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>25</v>
@@ -3325,16 +3327,16 @@
         <v>28</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>29</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>47</v>
@@ -3346,7 +3348,7 @@
         <v>16</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="L12" s="5"/>
       <c r="M12" s="11">
@@ -3369,7 +3371,7 @@
     </row>
     <row r="13" spans="1:22" ht="17" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>23</v>
@@ -3378,16 +3380,16 @@
         <v>27</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>29</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>47</v>
@@ -3399,7 +3401,7 @@
         <v>16</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="L13" s="5"/>
       <c r="M13" s="11">
@@ -3422,7 +3424,7 @@
     </row>
     <row r="14" spans="1:22" ht="17" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>24</v>
@@ -3431,16 +3433,16 @@
         <v>27</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>29</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>47</v>
@@ -3452,7 +3454,7 @@
         <v>16</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="L14" s="5"/>
       <c r="M14" s="11">
@@ -3475,7 +3477,7 @@
     </row>
     <row r="15" spans="1:22" ht="17" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>25</v>
@@ -3484,16 +3486,16 @@
         <v>27</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>29</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>47</v>
@@ -3505,7 +3507,7 @@
         <v>16</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="L15" s="5"/>
       <c r="M15" s="11">
@@ -3528,7 +3530,7 @@
     </row>
     <row r="16" spans="1:22" ht="17" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>23</v>
@@ -3537,16 +3539,16 @@
         <v>28</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>29</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>47</v>
@@ -3558,7 +3560,7 @@
         <v>16</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="L16" s="5"/>
       <c r="M16" s="11">
@@ -3581,7 +3583,7 @@
     </row>
     <row r="17" spans="1:21" ht="17" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>24</v>
@@ -3590,19 +3592,19 @@
         <v>28</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>29</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>47</v>
@@ -3614,7 +3616,7 @@
         <v>16</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="M17" s="5"/>
       <c r="N17" s="11">
@@ -3637,7 +3639,7 @@
     </row>
     <row r="18" spans="1:21" ht="17" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>26</v>
@@ -3646,19 +3648,19 @@
         <v>28</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>29</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>47</v>
@@ -3670,7 +3672,7 @@
         <v>16</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="M18" s="5"/>
       <c r="N18" s="11">
@@ -3694,7 +3696,7 @@
     <row r="19" spans="1:21" s="7" customFormat="1" ht="17" customHeight="1"/>
     <row r="20" spans="1:21" ht="17" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>20</v>
@@ -3703,19 +3705,19 @@
         <v>2</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>48</v>
@@ -3727,7 +3729,7 @@
         <v>16</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="M20" s="5"/>
       <c r="N20" s="11">
@@ -3750,7 +3752,7 @@
     </row>
     <row r="21" spans="1:21" ht="17" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>19</v>
@@ -3759,19 +3761,19 @@
         <v>2</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>48</v>
@@ -3783,7 +3785,7 @@
         <v>16</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="M21" s="5"/>
       <c r="N21" s="11">
@@ -3806,7 +3808,7 @@
     </row>
     <row r="22" spans="1:21" ht="17" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>6</v>
@@ -3815,19 +3817,19 @@
         <v>2</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>60</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>48</v>
@@ -3839,7 +3841,7 @@
         <v>3</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="M22" s="5"/>
       <c r="N22" s="11">
@@ -3862,7 +3864,7 @@
     </row>
     <row r="23" spans="1:21" ht="17" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>7</v>
@@ -3871,19 +3873,19 @@
         <v>2</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>60</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>48</v>
@@ -3895,7 +3897,7 @@
         <v>3</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="M23" s="5"/>
       <c r="N23" s="11">
@@ -3919,28 +3921,28 @@
     <row r="24" spans="1:21" s="7" customFormat="1" ht="17" customHeight="1"/>
     <row r="25" spans="1:21" ht="17" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>59</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I25" s="3" t="s">
         <v>49</v>
@@ -3952,7 +3954,7 @@
         <v>16</v>
       </c>
       <c r="L25" s="12" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="M25" s="3">
         <v>1</v>
@@ -3966,7 +3968,7 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="13" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="S25" s="1"/>
       <c r="T25" s="1">
@@ -3975,28 +3977,28 @@
     </row>
     <row r="26" spans="1:21" ht="17" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>59</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I26" s="3" t="s">
         <v>49</v>
@@ -4008,7 +4010,7 @@
         <v>16</v>
       </c>
       <c r="L26" s="12" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="M26" s="5">
         <v>1</v>
@@ -4020,7 +4022,7 @@
       </c>
       <c r="Q26" s="1"/>
       <c r="R26" s="13" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="S26" s="1"/>
       <c r="T26" s="1">
@@ -4029,28 +4031,28 @@
     </row>
     <row r="27" spans="1:21" ht="17" customHeight="1">
       <c r="A27" s="3" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>43</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I27" s="3" t="s">
         <v>50</v>
@@ -4062,7 +4064,7 @@
         <v>16</v>
       </c>
       <c r="L27" s="12" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="M27" s="3">
         <v>2</v>
@@ -4080,7 +4082,7 @@
         <v>42094</v>
       </c>
       <c r="R27" s="13" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="S27" s="1"/>
       <c r="T27" s="1">
@@ -4089,28 +4091,28 @@
     </row>
     <row r="28" spans="1:21" ht="17" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>43</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>51</v>
@@ -4122,7 +4124,7 @@
         <v>16</v>
       </c>
       <c r="L28" s="12" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="M28" s="3">
         <v>21</v>
@@ -4140,7 +4142,7 @@
         <v>42094</v>
       </c>
       <c r="R28" s="13" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="S28" s="1"/>
       <c r="T28" s="1">
@@ -4149,28 +4151,28 @@
     </row>
     <row r="29" spans="1:21" ht="17" customHeight="1">
       <c r="A29" s="3" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>44</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I29" s="3" t="s">
         <v>52</v>
@@ -4182,7 +4184,7 @@
         <v>16</v>
       </c>
       <c r="L29" s="12" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="M29" s="3">
         <v>7</v>
@@ -4200,7 +4202,7 @@
         <v>42094</v>
       </c>
       <c r="R29" s="13" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="S29" s="1"/>
       <c r="T29" s="1">
@@ -4209,28 +4211,28 @@
     </row>
     <row r="30" spans="1:21" ht="17" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>58</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>59</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I30" s="3" t="s">
         <v>49</v>
@@ -4242,7 +4244,7 @@
         <v>16</v>
       </c>
       <c r="L30" s="12" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="M30" s="3">
         <v>1</v>
@@ -4263,7 +4265,7 @@
     </row>
     <row r="31" spans="1:21" ht="17" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>32</v>
@@ -4272,19 +4274,19 @@
         <v>61</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>59</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I31" s="3" t="s">
         <v>63</v>
@@ -4296,7 +4298,7 @@
         <v>16</v>
       </c>
       <c r="L31" s="12" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="M31" s="3">
         <v>1</v>
@@ -4317,28 +4319,28 @@
     </row>
     <row r="32" spans="1:21" ht="17" customHeight="1">
       <c r="A32" s="3" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>62</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>69</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I32" s="3" t="s">
         <v>63</v>
@@ -4350,7 +4352,7 @@
         <v>16</v>
       </c>
       <c r="L32" s="12" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="M32" s="3">
         <v>1</v>
@@ -4373,28 +4375,28 @@
     </row>
     <row r="33" spans="1:21" ht="17" customHeight="1">
       <c r="A33" s="3" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>68</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>69</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I33" s="3" t="s">
         <v>63</v>
@@ -4406,7 +4408,7 @@
         <v>16</v>
       </c>
       <c r="L33" s="12" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="M33" s="3">
         <v>1</v>
@@ -4431,7 +4433,7 @@
     </row>
     <row r="34" spans="1:21" ht="17" customHeight="1">
       <c r="A34" s="3" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>38</v>
@@ -4449,10 +4451,10 @@
         <v>75</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I34" s="3" t="s">
         <v>76</v>
@@ -4464,7 +4466,7 @@
         <v>16</v>
       </c>
       <c r="L34" s="12" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="M34" s="4" t="s">
         <v>3</v>
@@ -4487,28 +4489,28 @@
     </row>
     <row r="35" spans="1:21" ht="17" customHeight="1">
       <c r="A35" s="3" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>77</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>78</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I35" s="3" t="s">
         <v>63</v>
@@ -4520,7 +4522,7 @@
         <v>16</v>
       </c>
       <c r="L35" s="12" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="M35" s="3">
         <v>1</v>
@@ -4541,7 +4543,7 @@
     </row>
     <row r="36" spans="1:21" ht="17" customHeight="1">
       <c r="A36" s="3" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>79</v>
@@ -4550,19 +4552,19 @@
         <v>70</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>69</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I36" s="8" t="s">
         <v>52</v>
@@ -4574,10 +4576,10 @@
         <v>16</v>
       </c>
       <c r="L36" s="12" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="M36" s="8" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="N36" s="11">
         <v>42185</v>
@@ -4595,28 +4597,28 @@
     </row>
     <row r="37" spans="1:21" ht="17" customHeight="1">
       <c r="A37" s="3" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>80</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>69</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I37" s="8" t="s">
         <v>52</v>
@@ -4628,10 +4630,10 @@
         <v>16</v>
       </c>
       <c r="L37" s="12" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="N37" s="11">
         <v>42277</v>
@@ -4649,7 +4651,7 @@
     </row>
     <row r="38" spans="1:21" ht="17" customHeight="1">
       <c r="A38" s="3" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>31</v>
@@ -4661,16 +4663,16 @@
         <v>55</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>56</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I38" s="3" t="s">
         <v>57</v>
@@ -4707,28 +4709,28 @@
     </row>
     <row r="39" spans="1:21" ht="17" customHeight="1">
       <c r="A39" s="3" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>82</v>
+        <v>260</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>81</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I39" s="3" t="s">
         <v>57</v>
@@ -4765,31 +4767,31 @@
     </row>
     <row r="40" spans="1:21" ht="17" customHeight="1">
       <c r="A40" s="3" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C40" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D40" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D40" s="6" t="s">
-        <v>84</v>
-      </c>
       <c r="E40" s="3" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="H40" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="I40" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="I40" s="6" t="s">
-        <v>99</v>
       </c>
       <c r="J40" s="4" t="s">
         <v>22</v>
@@ -4823,31 +4825,31 @@
     </row>
     <row r="41" spans="1:21" ht="17" customHeight="1">
       <c r="A41" s="3" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J41" s="4" t="s">
         <v>22</v>
@@ -4856,7 +4858,7 @@
         <v>16</v>
       </c>
       <c r="L41" s="12" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="M41" s="3" t="s">
         <v>72</v>
@@ -4877,31 +4879,31 @@
     </row>
     <row r="42" spans="1:21" ht="17" customHeight="1">
       <c r="A42" s="3" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J42" s="4" t="s">
         <v>22</v>
@@ -4910,7 +4912,7 @@
         <v>16</v>
       </c>
       <c r="L42" s="12" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="M42" s="3">
         <v>2</v>
@@ -4931,28 +4933,28 @@
     </row>
     <row r="43" spans="1:21" ht="17" customHeight="1">
       <c r="A43" s="3" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I43" s="3" t="s">
         <v>47</v>
@@ -4964,7 +4966,7 @@
         <v>16</v>
       </c>
       <c r="L43" s="12" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="M43" s="3" t="s">
         <v>72</v>
@@ -4985,25 +4987,25 @@
     </row>
     <row r="44" spans="1:21" ht="17" customHeight="1">
       <c r="A44" s="3" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>22</v>
       </c>
       <c r="G44" s="15" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="H44" s="4" t="s">
         <v>22</v>
@@ -5018,7 +5020,7 @@
         <v>16</v>
       </c>
       <c r="L44" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M44" s="15">
         <v>1</v>
@@ -5040,31 +5042,31 @@
     <row r="45" spans="1:21" s="7" customFormat="1" ht="17" customHeight="1"/>
     <row r="46" spans="1:21" ht="17" customHeight="1">
       <c r="A46" s="3" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="F46" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="I46" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="I46" s="3" t="s">
-        <v>117</v>
       </c>
       <c r="J46" s="3">
         <v>3</v>
@@ -5073,7 +5075,7 @@
         <v>16</v>
       </c>
       <c r="L46" s="16" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="M46" s="3">
         <v>100</v>
@@ -5098,28 +5100,28 @@
     </row>
     <row r="47" spans="1:21" ht="17" customHeight="1">
       <c r="A47" s="3" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I47" s="3" t="s">
         <v>52</v>
@@ -5131,7 +5133,7 @@
         <v>16</v>
       </c>
       <c r="L47" s="16" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="M47" s="3">
         <v>100</v>
@@ -5154,46 +5156,46 @@
         <v>2</v>
       </c>
       <c r="U47" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="48" spans="1:21" s="7" customFormat="1" ht="17" customHeight="1"/>
     <row r="49" spans="1:25" ht="17" customHeight="1">
       <c r="A49" s="3" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="H49" s="4" t="s">
         <v>22</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="J49" s="3">
         <v>2</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L49" s="3" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="M49" s="3">
         <v>3</v>
@@ -5216,40 +5218,40 @@
     </row>
     <row r="50" spans="1:25" ht="17" customHeight="1">
       <c r="A50" s="3" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="H50" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="J50" s="3">
+        <v>2</v>
+      </c>
+      <c r="K50" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="I50" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="J50" s="3">
-        <v>2</v>
-      </c>
-      <c r="K50" s="3" t="s">
-        <v>135</v>
-      </c>
       <c r="L50" s="3" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="M50" s="3">
         <v>2</v>
@@ -5272,28 +5274,28 @@
     </row>
     <row r="51" spans="1:25" ht="17" customHeight="1">
       <c r="A51" s="3" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="I51" s="3" t="s">
         <v>52</v>
@@ -5302,10 +5304,10 @@
         <v>2</v>
       </c>
       <c r="K51" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="L51" s="3" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="M51" s="3">
         <v>3</v>
@@ -5328,25 +5330,25 @@
     </row>
     <row r="52" spans="1:25" ht="17" customHeight="1">
       <c r="A52" s="3" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>126</v>
+        <v>261</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="H52" s="4" t="s">
         <v>22</v>
@@ -5361,7 +5363,7 @@
         <v>22</v>
       </c>
       <c r="L52" s="3" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="M52" s="3">
         <v>1</v>
@@ -5384,25 +5386,25 @@
     </row>
     <row r="53" spans="1:25" ht="17" customHeight="1">
       <c r="A53" s="3" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="H53" s="4" t="s">
         <v>22</v>
@@ -5417,7 +5419,7 @@
         <v>22</v>
       </c>
       <c r="L53" s="3" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="M53" s="3">
         <v>1</v>
@@ -5440,25 +5442,25 @@
     </row>
     <row r="54" spans="1:25" ht="17" customHeight="1">
       <c r="A54" s="3" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>128</v>
+        <v>262</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="H54" s="4" t="s">
         <v>22</v>
@@ -5473,7 +5475,7 @@
         <v>22</v>
       </c>
       <c r="L54" s="3" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="M54" s="3">
         <v>1</v>
@@ -5496,25 +5498,25 @@
     </row>
     <row r="55" spans="1:25" ht="17" customHeight="1">
       <c r="A55" s="3" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>148</v>
+        <v>263</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="H55" s="4" t="s">
         <v>22</v>
@@ -5529,7 +5531,7 @@
         <v>22</v>
       </c>
       <c r="L55" s="3" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="M55" s="3">
         <v>1</v>
@@ -5550,25 +5552,25 @@
     </row>
     <row r="56" spans="1:25" ht="17" customHeight="1">
       <c r="A56" s="3" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>153</v>
+        <v>264</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>151</v>
+        <v>265</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="H56" s="4" t="s">
         <v>22</v>
@@ -5583,7 +5585,7 @@
         <v>22</v>
       </c>
       <c r="L56" s="3" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="M56" s="3">
         <v>1</v>
@@ -5606,25 +5608,25 @@
     </row>
     <row r="57" spans="1:25" ht="17" customHeight="1">
       <c r="A57" s="3" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>154</v>
+        <v>266</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>150</v>
+        <v>267</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="H57" s="4" t="s">
         <v>22</v>
@@ -5639,7 +5641,7 @@
         <v>22</v>
       </c>
       <c r="L57" s="3" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="M57" s="3">
         <v>1</v>
@@ -5662,25 +5664,25 @@
     </row>
     <row r="58" spans="1:25" ht="17" customHeight="1">
       <c r="A58" s="3" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="H58" s="4" t="s">
         <v>22</v>
@@ -5695,7 +5697,7 @@
         <v>22</v>
       </c>
       <c r="L58" s="3" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="M58" s="3">
         <v>1</v>
@@ -5718,25 +5720,25 @@
     </row>
     <row r="59" spans="1:25" ht="17" customHeight="1">
       <c r="A59" s="3" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="H59" s="4" t="s">
         <v>22</v>
@@ -5751,7 +5753,7 @@
         <v>22</v>
       </c>
       <c r="L59" s="3" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="M59" s="3">
         <v>3</v>
@@ -5774,25 +5776,25 @@
     </row>
     <row r="60" spans="1:25" ht="17" customHeight="1">
       <c r="A60" s="3" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>157</v>
+        <v>268</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="H60" s="4" t="s">
         <v>22</v>
@@ -5807,7 +5809,7 @@
         <v>22</v>
       </c>
       <c r="L60" s="3" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="M60" s="3">
         <v>3</v>
@@ -5830,25 +5832,25 @@
     </row>
     <row r="61" spans="1:25" ht="17" customHeight="1">
       <c r="A61" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="B61" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>158</v>
-      </c>
       <c r="D61" s="3" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="H61" s="4" t="s">
         <v>22</v>
@@ -5863,7 +5865,7 @@
         <v>22</v>
       </c>
       <c r="L61" s="3" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="M61" s="3">
         <v>3</v>
@@ -5887,25 +5889,25 @@
     <row r="62" spans="1:25" s="7" customFormat="1" ht="17" customHeight="1"/>
     <row r="63" spans="1:25" ht="17" customHeight="1">
       <c r="A63" s="17" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>138</v>
+        <v>270</v>
       </c>
       <c r="D63" s="17" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="E63" s="17" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="F63" s="17" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G63" s="17" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="H63" s="18" t="s">
         <v>22</v>
@@ -5920,7 +5922,7 @@
         <v>16</v>
       </c>
       <c r="L63" s="17" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="M63" s="17">
         <v>13</v>
@@ -5950,25 +5952,25 @@
     </row>
     <row r="64" spans="1:25" ht="17" customHeight="1">
       <c r="A64" s="17" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>138</v>
+        <v>270</v>
       </c>
       <c r="D64" s="17" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="E64" s="17" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="F64" s="17" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G64" s="17" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="H64" s="18" t="s">
         <v>22</v>
@@ -5983,7 +5985,7 @@
         <v>16</v>
       </c>
       <c r="L64" s="17" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="M64" s="17">
         <v>13</v>

</xml_diff>

<commit_message>
Revised the Center names and corrected minor typographical errors
</commit_message>
<xml_diff>
--- a/milestones-consolidated.xlsx
+++ b/milestones-consolidated.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-1860" yWindow="-16000" windowWidth="25520" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="-1860" yWindow="-15998" windowWidth="25523" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,6 @@
     <t>TBD</t>
   </si>
   <si>
-    <t>purturbagens</t>
-  </si>
-  <si>
     <t>cell-lines</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t>perturbagens-meta</t>
   </si>
   <si>
-    <t>name1,type1,perturbagens1;name2,type2, purturbagens2</t>
-  </si>
-  <si>
     <t>evaluating CRISPRs (vs shRNAs)</t>
   </si>
   <si>
@@ -135,9 +129,6 @@
     <t>BRAF6: Phosphorylation state and levels of ~24 transcription factors measured in BRAF(V600E/D) melanoma cell lines monitored by imaging</t>
   </si>
   <si>
-    <t>LJP 5&amp;6-growth inhibition/drug combinations: Sensitivity measures of 6 breast cancer cell lines to combination treatment of kinase inhibitors based on results of  dataset LJP5&amp;6-growth inhibition/single drugs</t>
-  </si>
-  <si>
     <t>MassSpecPhos1: Basal profiling of phosphoproteins measured by mass spec</t>
   </si>
   <si>
@@ -258,9 +249,6 @@
     <t>177 compounds,small molecules</t>
   </si>
   <si>
-    <t>Breast Cancer HCI1: High content images of 4 breast cancer cell lines treated with 106 kinase inhibitors (plates LJP5-6);collaboration with the David Andrews lab (University of Toronto)</t>
-  </si>
-  <si>
     <t>Imaging assay--2 cell lines treated with 3 different doses of the LJP5&amp;6 plates of kinase inhibitors. Cells will be  stained with TMRE (mitochondria) and DRAQ5 (DNA/nuclei). Intensity, mophology and texture features will be extracted at the well and single cell levels.</t>
   </si>
   <si>
@@ -486,9 +474,6 @@
     <t>Nuclei/cell count\image;Apoptotic cells\image</t>
   </si>
   <si>
-    <t>p27 Kip1--Alexa488\image;p-Histone H3(S10)--Alexa488\image;Ki-67--Alexa488\image;p-Rb(S807/S811)--Alexa568\image;p-ERK(T202/Y204)--Alexa647\image;p-S6(S235/S236--Alexa647\image;p-cJun(S73)--Alexa647\image</t>
-  </si>
-  <si>
     <t>Intensity, mophology and texture features (300+ features total)\image</t>
   </si>
   <si>
@@ -675,9 +660,6 @@
     <t>&gt;300</t>
   </si>
   <si>
-    <t>LJP 5&amp;6-L1000/single drugs: L1000 response of 6 breast cancer cell lines to treatment plates LJP5&amp;6 (106 kinase inhibitors)</t>
-  </si>
-  <si>
     <t>pMEK(S217/221)\phosphorylation level;pERK(T202/Y204)\phosphorylation level;p-p90RSK(S380)\phosphorylation level;p-p90RSK(T573)\phosphorylation level;p-AKT(T308)\phosphorylation level;p-AKT(S473)\phosphorylation level;p-mTOR(S2448)\phosphorylation level;p-p70S6K(T421/S424)\phosphorylation level;p-p70S6K(T389)\phosphorylation level;p-S6(S235/236)\phosphorylation level;p-AMPK(T172)\phosphorylation level;p-JNK(T183/Y185)\phosphorylation level;Total c-Jun\phosphorylation level;p-cJun(S63)\phosphorylation level;p-P38(T180/Y182)\phosphorylation level;p-HSP27(S82)\phosphorylation level;p-NFKB(S536)\phosphorylation level;Bim\phosphorylation level;cPARP\phosphorylation level;p-Histone H3(S10)\phosphorylation level;p27 Kip1\phosphorylation level</t>
   </si>
   <si>
@@ -732,12 +714,6 @@
     <t>L1000 gene expression\number</t>
   </si>
   <si>
-    <t>LJP 5&amp;6-growth inhibition/single drugs: Sensitivity measures of 6 breast cancer cell lines to treatment plates LJP5&amp;6 (106 kinase inhibitors); complement to dataset LJP5&amp;6-L1000/single drugs</t>
-  </si>
-  <si>
-    <t>LJP 5&amp;6-L1000/drug combinations: L1000 response of 6 breast cancer cell lines to treatment plates LJP7-9 (177 targeted drugs). Complement  to dataset LJP5&amp;6-L1000/single drugs</t>
-  </si>
-  <si>
     <t>Breast Cancer HCI2: High content images of 2 breast cancer cell lines treated with 106 kinase inhibitors (plates LJP5-6); complement to dataset Breast cancer HCI1</t>
   </si>
   <si>
@@ -780,21 +756,6 @@
     <t>name1,type1(cell line or iPSC differentiated),class1(cell line,cancer line,…)\control-or-disease,tissue1;name2,type2,class2,tissue2</t>
   </si>
   <si>
-    <t>DTOXS</t>
-  </si>
-  <si>
-    <t>HMS-LINCS</t>
-  </si>
-  <si>
-    <t>Broad-LINCS-Transcriptomics</t>
-  </si>
-  <si>
-    <t>Broad-LINCS-PCCSE</t>
-  </si>
-  <si>
-    <t>MEP-LINCS</t>
-  </si>
-  <si>
     <t>NeuroLINCS</t>
   </si>
   <si>
@@ -832,13 +793,52 @@
   </si>
   <si>
     <t>Use microenvironment microarray (MEMA) based platform to assess the impacts of ~3000 different pairwise combinations of ME perturbagens (MEPs) on 10 biological response endpoints.</t>
+  </si>
+  <si>
+    <t>p27 Kip1--Alexa488\image;p-Histone H3(S10)--Alexa488\image;Ki-67--Alexa488\image;p-Rb(S807/S811)--Alexa568\image;p-ERK(T202/Y204)--Alexa647\image;p-S6(S235/S236)--Alexa647\image;p-cJun(S73)--Alexa647\image</t>
+  </si>
+  <si>
+    <t>name1,type1,perturbagens1;name2,type2, perturbagens2</t>
+  </si>
+  <si>
+    <t>perturbagens</t>
+  </si>
+  <si>
+    <t>LJP5&amp;6-L1000/single drugs: L1000 response of 6 breast cancer cell lines to treatment plates LJP5&amp;6 (106 kinase inhibitors)</t>
+  </si>
+  <si>
+    <t>LJP5&amp;6-growth inhibition/single drugs: Sensitivity measures of 6 breast cancer cell lines to treatment plates LJP5&amp;6 (106 kinase inhibitors); complement to dataset LJP5&amp;6-L1000/single drugs</t>
+  </si>
+  <si>
+    <t>LJP5&amp;6-growth inhibition/drug combinations: Sensitivity measures of 6 breast cancer cell lines to combination treatment of kinase inhibitors based on results of  dataset LJP5&amp;6-growth inhibition/single drugs</t>
+  </si>
+  <si>
+    <t>LJP5&amp;6-L1000/drug combinations: L1000 response of 6 breast cancer cell lines to treatment plates LJP7-9 (177 targeted drugs). Complement  to dataset LJP5&amp;6-L1000/single drugs</t>
+  </si>
+  <si>
+    <t>LINCS Proteomic Characterization Center</t>
+  </si>
+  <si>
+    <t>HMS LINCS</t>
+  </si>
+  <si>
+    <t>DToxS</t>
+  </si>
+  <si>
+    <t>LINCS Center for Transcriptomics</t>
+  </si>
+  <si>
+    <t>MEP LINCS</t>
+  </si>
+  <si>
+    <t>Breast Cancer HCI1: High content images of 4 breast cancer cell lines treated with 106 kinase inhibitors (plates LJP5-6); collaboration with the David Andrews lab (University of Toronto)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2737,14 +2737,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="17" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="28.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="105.5" style="3" customWidth="1"/>
+    <col min="1" max="1" width="46" style="3" customWidth="1"/>
+    <col min="2" max="2" width="145.875" style="3" customWidth="1"/>
     <col min="3" max="3" width="23" style="3" customWidth="1"/>
     <col min="4" max="4" width="142" style="3" customWidth="1"/>
     <col min="5" max="5" width="31.875" style="3" customWidth="1"/>
@@ -2766,45 +2766,45 @@
     <col min="23" max="16384" width="10.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="2" customFormat="1" ht="32">
+    <row r="1" spans="1:22" s="2" customFormat="1" ht="31.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="L1" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>1</v>
@@ -2819,103 +2819,103 @@
         <v>1</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="V1" s="10"/>
     </row>
     <row r="2" spans="1:22" s="2" customFormat="1" ht="17" customHeight="1">
       <c r="D2" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>18</v>
+        <v>259</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="L2" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="S2" s="2" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="V2" s="10"/>
     </row>
     <row r="3" spans="1:22" s="2" customFormat="1" ht="17" customHeight="1">
       <c r="K3" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="V3" s="10"/>
     </row>
     <row r="4" spans="1:22" ht="17" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J4" s="3">
         <v>3</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="M4" s="5"/>
       <c r="N4" s="11">
@@ -2937,40 +2937,40 @@
     </row>
     <row r="5" spans="1:22" ht="17" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J5" s="3">
         <v>3</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="M5" s="5"/>
       <c r="N5" s="11">
@@ -2992,40 +2992,40 @@
     </row>
     <row r="6" spans="1:22" ht="17" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J6" s="3">
         <v>3</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="M6" s="5"/>
       <c r="N6" s="11">
@@ -3047,40 +3047,40 @@
     </row>
     <row r="7" spans="1:22" ht="17" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J7" s="3">
         <v>3</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="M7" s="5"/>
       <c r="N7" s="11">
@@ -3103,40 +3103,40 @@
     </row>
     <row r="8" spans="1:22" ht="17" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J8" s="3">
         <v>3</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="M8" s="5"/>
       <c r="N8" s="11">
@@ -3159,37 +3159,37 @@
     </row>
     <row r="9" spans="1:22" ht="17" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I9" s="3">
         <v>3</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="L9" s="5"/>
       <c r="M9" s="11">
@@ -3212,50 +3212,50 @@
     </row>
     <row r="10" spans="1:22" ht="17" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I10" s="3">
         <v>3</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="L10" s="5"/>
       <c r="M10" s="11">
-        <v>42292</v>
+        <v>42308</v>
       </c>
       <c r="N10" s="11">
-        <v>42292</v>
+        <v>42308</v>
       </c>
       <c r="O10" s="11">
-        <v>42292</v>
+        <v>42308</v>
       </c>
       <c r="P10" s="11">
-        <v>42292</v>
+        <v>42308</v>
       </c>
       <c r="Q10" s="11"/>
       <c r="T10" s="3">
@@ -3265,50 +3265,50 @@
     </row>
     <row r="11" spans="1:22" ht="17" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I11" s="3">
         <v>3</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="11">
-        <v>42292</v>
+        <v>42308</v>
       </c>
       <c r="N11" s="11">
-        <v>42292</v>
+        <v>42308</v>
       </c>
       <c r="O11" s="11">
-        <v>42292</v>
+        <v>42308</v>
       </c>
       <c r="P11" s="11">
-        <v>42292</v>
+        <v>42308</v>
       </c>
       <c r="Q11" s="11"/>
       <c r="T11" s="3">
@@ -3318,50 +3318,50 @@
     </row>
     <row r="12" spans="1:22" ht="17" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I12" s="3">
         <v>3</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="L12" s="5"/>
       <c r="M12" s="11">
-        <v>42292</v>
+        <v>42308</v>
       </c>
       <c r="N12" s="11">
-        <v>42292</v>
+        <v>42308</v>
       </c>
       <c r="O12" s="11">
-        <v>42292</v>
+        <v>42308</v>
       </c>
       <c r="P12" s="11">
-        <v>42292</v>
+        <v>42308</v>
       </c>
       <c r="Q12" s="11"/>
       <c r="T12" s="3">
@@ -3371,50 +3371,50 @@
     </row>
     <row r="13" spans="1:22" ht="17" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="F13" s="3" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="L13" s="5"/>
       <c r="M13" s="11">
-        <v>42292</v>
+        <v>42308</v>
       </c>
       <c r="N13" s="11">
-        <v>42292</v>
+        <v>42308</v>
       </c>
       <c r="O13" s="11">
-        <v>42292</v>
+        <v>42308</v>
       </c>
       <c r="P13" s="11">
-        <v>42292</v>
+        <v>42308</v>
       </c>
       <c r="Q13" s="11"/>
       <c r="T13" s="3">
@@ -3424,50 +3424,50 @@
     </row>
     <row r="14" spans="1:22" ht="17" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="F14" s="3" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="L14" s="5"/>
       <c r="M14" s="11">
-        <v>42292</v>
+        <v>42308</v>
       </c>
       <c r="N14" s="11">
-        <v>42292</v>
+        <v>42308</v>
       </c>
       <c r="O14" s="11">
-        <v>42292</v>
+        <v>42308</v>
       </c>
       <c r="P14" s="11">
-        <v>42292</v>
+        <v>42308</v>
       </c>
       <c r="Q14" s="11"/>
       <c r="T14" s="3">
@@ -3477,50 +3477,50 @@
     </row>
     <row r="15" spans="1:22" ht="17" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="F15" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="L15" s="5"/>
       <c r="M15" s="11">
-        <v>42292</v>
+        <v>42308</v>
       </c>
       <c r="N15" s="11">
-        <v>42292</v>
+        <v>42308</v>
       </c>
       <c r="O15" s="11">
-        <v>42292</v>
+        <v>42308</v>
       </c>
       <c r="P15" s="11">
-        <v>42292</v>
+        <v>42308</v>
       </c>
       <c r="Q15" s="11"/>
       <c r="T15" s="3">
@@ -3530,37 +3530,37 @@
     </row>
     <row r="16" spans="1:22" ht="17" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I16" s="3">
         <v>3</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="L16" s="5"/>
       <c r="M16" s="11">
@@ -3583,40 +3583,40 @@
     </row>
     <row r="17" spans="1:21" ht="17" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J17" s="3">
         <v>3</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="M17" s="5"/>
       <c r="N17" s="11">
@@ -3639,40 +3639,40 @@
     </row>
     <row r="18" spans="1:21" ht="17" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="D18" s="3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J18" s="3">
         <v>3</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="M18" s="5"/>
       <c r="N18" s="11">
@@ -3696,40 +3696,40 @@
     <row r="19" spans="1:21" s="7" customFormat="1" ht="17" customHeight="1"/>
     <row r="20" spans="1:21" ht="17" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>255</v>
+        <v>268</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J20" s="3">
         <v>3</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="M20" s="5"/>
       <c r="N20" s="11">
@@ -3752,40 +3752,40 @@
     </row>
     <row r="21" spans="1:21" ht="17" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>255</v>
+        <v>268</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J21" s="3">
         <v>3</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="M21" s="5"/>
       <c r="N21" s="11">
@@ -3808,31 +3808,31 @@
     </row>
     <row r="22" spans="1:21" ht="17" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>255</v>
+        <v>268</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J22" s="3">
         <v>3</v>
@@ -3841,7 +3841,7 @@
         <v>3</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="M22" s="5"/>
       <c r="N22" s="11">
@@ -3864,31 +3864,31 @@
     </row>
     <row r="23" spans="1:21" ht="17" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>255</v>
+        <v>268</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J23" s="3">
         <v>3</v>
@@ -3897,7 +3897,7 @@
         <v>3</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="M23" s="5"/>
       <c r="N23" s="11">
@@ -3921,40 +3921,40 @@
     <row r="24" spans="1:21" s="7" customFormat="1" ht="17" customHeight="1"/>
     <row r="25" spans="1:21" ht="17" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L25" s="12" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="M25" s="3">
         <v>1</v>
@@ -3968,7 +3968,7 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="13" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="S25" s="1"/>
       <c r="T25" s="1">
@@ -3977,40 +3977,40 @@
     </row>
     <row r="26" spans="1:21" ht="17" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L26" s="12" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="M26" s="5">
         <v>1</v>
@@ -4022,7 +4022,7 @@
       </c>
       <c r="Q26" s="1"/>
       <c r="R26" s="13" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="S26" s="1"/>
       <c r="T26" s="1">
@@ -4031,40 +4031,40 @@
     </row>
     <row r="27" spans="1:21" ht="17" customHeight="1">
       <c r="A27" s="3" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L27" s="12" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="M27" s="3">
         <v>2</v>
@@ -4082,7 +4082,7 @@
         <v>42094</v>
       </c>
       <c r="R27" s="13" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="S27" s="1"/>
       <c r="T27" s="1">
@@ -4091,40 +4091,40 @@
     </row>
     <row r="28" spans="1:21" ht="17" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L28" s="12" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="M28" s="3">
         <v>21</v>
@@ -4142,7 +4142,7 @@
         <v>42094</v>
       </c>
       <c r="R28" s="13" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="S28" s="1"/>
       <c r="T28" s="1">
@@ -4151,40 +4151,40 @@
     </row>
     <row r="29" spans="1:21" ht="17" customHeight="1">
       <c r="A29" s="3" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L29" s="12" t="s">
-        <v>155</v>
+        <v>258</v>
       </c>
       <c r="M29" s="3">
         <v>7</v>
@@ -4202,7 +4202,7 @@
         <v>42094</v>
       </c>
       <c r="R29" s="13" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="S29" s="1"/>
       <c r="T29" s="1">
@@ -4211,40 +4211,40 @@
     </row>
     <row r="30" spans="1:21" ht="17" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L30" s="12" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="M30" s="3">
         <v>1</v>
@@ -4265,40 +4265,40 @@
     </row>
     <row r="31" spans="1:21" ht="17" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L31" s="12" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="M31" s="3">
         <v>1</v>
@@ -4319,40 +4319,40 @@
     </row>
     <row r="32" spans="1:21" ht="17" customHeight="1">
       <c r="A32" s="3" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>218</v>
+        <v>261</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L32" s="12" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="M32" s="3">
         <v>1</v>
@@ -4375,40 +4375,40 @@
     </row>
     <row r="33" spans="1:21" ht="17" customHeight="1">
       <c r="A33" s="3" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>237</v>
+        <v>262</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L33" s="12" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="M33" s="3">
         <v>1</v>
@@ -4433,40 +4433,40 @@
     </row>
     <row r="34" spans="1:21" ht="17" customHeight="1">
       <c r="A34" s="3" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>38</v>
+        <v>263</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L34" s="12" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="M34" s="4" t="s">
         <v>3</v>
@@ -4489,40 +4489,40 @@
     </row>
     <row r="35" spans="1:21" ht="17" customHeight="1">
       <c r="A35" s="3" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>238</v>
+        <v>264</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L35" s="12" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="M35" s="3">
         <v>1</v>
@@ -4543,43 +4543,43 @@
     </row>
     <row r="36" spans="1:21" ht="17" customHeight="1">
       <c r="A36" s="3" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>79</v>
+        <v>270</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L36" s="12" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="M36" s="8" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="N36" s="11">
         <v>42185</v>
@@ -4597,43 +4597,43 @@
     </row>
     <row r="37" spans="1:21" ht="17" customHeight="1">
       <c r="A37" s="3" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L37" s="12" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="N37" s="11">
         <v>42277</v>
@@ -4651,40 +4651,40 @@
     </row>
     <row r="38" spans="1:21" ht="17" customHeight="1">
       <c r="A38" s="3" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C38" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I38" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D38" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="J38" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L38" s="12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M38" s="5">
         <v>51</v>
@@ -4709,40 +4709,40 @@
     </row>
     <row r="39" spans="1:21" ht="17" customHeight="1">
       <c r="A39" s="3" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L39" s="12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M39" s="3">
         <v>51</v>
@@ -4767,40 +4767,40 @@
     </row>
     <row r="40" spans="1:21" ht="17" customHeight="1">
       <c r="A40" s="3" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L40" s="12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M40" s="3">
         <v>51</v>
@@ -4825,43 +4825,43 @@
     </row>
     <row r="41" spans="1:21" ht="17" customHeight="1">
       <c r="A41" s="3" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C41" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="H41" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="H41" s="3" t="s">
+      <c r="I41" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="I41" s="6" t="s">
-        <v>107</v>
-      </c>
       <c r="J41" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L41" s="12" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N41" s="11">
         <v>42369</v>
@@ -4879,40 +4879,40 @@
     </row>
     <row r="42" spans="1:21" ht="17" customHeight="1">
       <c r="A42" s="3" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L42" s="12" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="M42" s="3">
         <v>2</v>
@@ -4933,43 +4933,43 @@
     </row>
     <row r="43" spans="1:21" ht="17" customHeight="1">
       <c r="A43" s="3" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L43" s="12" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N43" s="11">
         <v>42369</v>
@@ -4987,40 +4987,40 @@
     </row>
     <row r="44" spans="1:21" ht="17" customHeight="1">
       <c r="A44" s="3" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G44" s="15" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L44" s="12" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="M44" s="15">
         <v>1</v>
@@ -5042,40 +5042,40 @@
     <row r="45" spans="1:21" s="7" customFormat="1" ht="17" customHeight="1"/>
     <row r="46" spans="1:21" ht="17" customHeight="1">
       <c r="A46" s="3" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C46" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I46" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="I46" s="3" t="s">
-        <v>116</v>
       </c>
       <c r="J46" s="3">
         <v>3</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L46" s="16" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="M46" s="3">
         <v>100</v>
@@ -5100,40 +5100,40 @@
     </row>
     <row r="47" spans="1:21" ht="17" customHeight="1">
       <c r="A47" s="3" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="B47" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F47" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>115</v>
-      </c>
       <c r="G47" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J47" s="3">
         <v>3</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L47" s="16" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="M47" s="3">
         <v>100</v>
@@ -5156,46 +5156,46 @@
         <v>2</v>
       </c>
       <c r="U47" s="6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:21" s="7" customFormat="1" ht="17" customHeight="1"/>
     <row r="49" spans="1:25" ht="17" customHeight="1">
       <c r="A49" s="3" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I49" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="J49" s="3">
+        <v>2</v>
+      </c>
+      <c r="K49" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="J49" s="3">
-        <v>2</v>
-      </c>
-      <c r="K49" s="3" t="s">
-        <v>131</v>
-      </c>
       <c r="L49" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="M49" s="3">
         <v>3</v>
@@ -5218,40 +5218,40 @@
     </row>
     <row r="50" spans="1:25" ht="17" customHeight="1">
       <c r="A50" s="3" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="I50" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="J50" s="3">
+        <v>2</v>
+      </c>
+      <c r="K50" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="J50" s="3">
-        <v>2</v>
-      </c>
-      <c r="K50" s="3" t="s">
-        <v>132</v>
-      </c>
       <c r="L50" s="3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="M50" s="3">
         <v>2</v>
@@ -5274,40 +5274,40 @@
     </row>
     <row r="51" spans="1:25" ht="17" customHeight="1">
       <c r="A51" s="3" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J51" s="3">
         <v>2</v>
       </c>
       <c r="K51" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="L51" s="3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="M51" s="3">
         <v>3</v>
@@ -5330,40 +5330,40 @@
     </row>
     <row r="52" spans="1:25" ht="17" customHeight="1">
       <c r="A52" s="3" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K52" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L52" s="3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="M52" s="3">
         <v>1</v>
@@ -5386,40 +5386,40 @@
     </row>
     <row r="53" spans="1:25" ht="17" customHeight="1">
       <c r="A53" s="3" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="B53" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="F53" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C53" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>126</v>
-      </c>
       <c r="G53" s="3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K53" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L53" s="3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="M53" s="3">
         <v>1</v>
@@ -5442,40 +5442,40 @@
     </row>
     <row r="54" spans="1:25" ht="17" customHeight="1">
       <c r="A54" s="3" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K54" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L54" s="3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="M54" s="3">
         <v>1</v>
@@ -5498,40 +5498,40 @@
     </row>
     <row r="55" spans="1:25" ht="17" customHeight="1">
       <c r="A55" s="3" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K55" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L55" s="3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="M55" s="3">
         <v>1</v>
@@ -5552,40 +5552,40 @@
     </row>
     <row r="56" spans="1:25" ht="17" customHeight="1">
       <c r="A56" s="3" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K56" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L56" s="3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="M56" s="3">
         <v>1</v>
@@ -5608,40 +5608,40 @@
     </row>
     <row r="57" spans="1:25" ht="17" customHeight="1">
       <c r="A57" s="3" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K57" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L57" s="3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="M57" s="3">
         <v>1</v>
@@ -5664,40 +5664,40 @@
     </row>
     <row r="58" spans="1:25" ht="17" customHeight="1">
       <c r="A58" s="3" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K58" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L58" s="3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="M58" s="3">
         <v>1</v>
@@ -5720,40 +5720,40 @@
     </row>
     <row r="59" spans="1:25" ht="17" customHeight="1">
       <c r="A59" s="3" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J59" s="3">
         <v>3</v>
       </c>
       <c r="K59" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L59" s="3" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="M59" s="3">
         <v>3</v>
@@ -5776,40 +5776,40 @@
     </row>
     <row r="60" spans="1:25" ht="17" customHeight="1">
       <c r="A60" s="3" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J60" s="3">
         <v>3</v>
       </c>
       <c r="K60" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L60" s="3" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="M60" s="3">
         <v>3</v>
@@ -5832,40 +5832,40 @@
     </row>
     <row r="61" spans="1:25" ht="17" customHeight="1">
       <c r="A61" s="3" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J61" s="3">
         <v>3</v>
       </c>
       <c r="K61" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L61" s="3" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="M61" s="3">
         <v>3</v>
@@ -5889,40 +5889,40 @@
     <row r="62" spans="1:25" s="7" customFormat="1" ht="17" customHeight="1"/>
     <row r="63" spans="1:25" ht="17" customHeight="1">
       <c r="A63" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="B63" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="C63" s="17" t="s">
         <v>257</v>
       </c>
-      <c r="B63" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="C63" s="17" t="s">
-        <v>270</v>
-      </c>
       <c r="D63" s="17" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E63" s="17" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="F63" s="17" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G63" s="17" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="H63" s="18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I63" s="18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J63" s="17">
         <v>6</v>
       </c>
       <c r="K63" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L63" s="17" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="M63" s="17">
         <v>13</v>
@@ -5952,40 +5952,40 @@
     </row>
     <row r="64" spans="1:25" ht="17" customHeight="1">
       <c r="A64" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="B64" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="C64" s="17" t="s">
         <v>257</v>
       </c>
-      <c r="B64" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="C64" s="17" t="s">
-        <v>270</v>
-      </c>
       <c r="D64" s="17" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E64" s="17" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="F64" s="17" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G64" s="17" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="H64" s="18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I64" s="18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J64" s="17">
         <v>6</v>
       </c>
       <c r="K64" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L64" s="17" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="M64" s="17">
         <v>13</v>

</xml_diff>